<commit_message>
Calibration 2010-2020; Biofuel chain; Heat generation and solar thermal technologies
Calibration for energy supply by source and type (where available, i.e. for oil and coal), energy consumption by fuel and sector, imports/exports, electricity generation by source and CO2 emissions by sector. Biofuel production chain from JRC-EU TIMES Model; Heat generation and solar thermal technologies
</commit_message>
<xml_diff>
--- a/TEMOA_Europe_Results/_1_Transport_fueltechs.xlsx
+++ b/TEMOA_Europe_Results/_1_Transport_fueltechs.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="62">
   <si>
     <t>tech</t>
   </si>
@@ -50,60 +50,117 @@
     <t>2050</t>
   </si>
   <si>
+    <t>TRA_FT_COA</t>
+  </si>
+  <si>
+    <t>TRA_FT_AVG</t>
+  </si>
+  <si>
+    <t>TRA_FT_DST</t>
+  </si>
+  <si>
+    <t>TRA_FT_ELC</t>
+  </si>
+  <si>
+    <t>TRA_FT_GSL</t>
+  </si>
+  <si>
+    <t>TRA_FT_HFO</t>
+  </si>
+  <si>
+    <t>TRA_FT_LPG</t>
+  </si>
+  <si>
+    <t>TRA_FT_NGA</t>
+  </si>
+  <si>
+    <t>TRA_FT_LNG</t>
+  </si>
+  <si>
+    <t>TRA_FT_ETH</t>
+  </si>
+  <si>
+    <t>TRA_FT_AMM_ELCSYS_CU</t>
+  </si>
+  <si>
+    <t>TRA_FT_AMM_ELCSYS_DT</t>
+  </si>
+  <si>
+    <t>TRA_FT_MTH</t>
+  </si>
+  <si>
+    <t>PRI_COA_HCO</t>
+  </si>
+  <si>
+    <t>PRI_COA_BCO</t>
+  </si>
+  <si>
+    <t>PRI_OIL_JTG</t>
+  </si>
+  <si>
+    <t>PRI_OIL_DST_kt</t>
+  </si>
+  <si>
+    <t>RNW_BIO_EMHV</t>
+  </si>
+  <si>
+    <t>RNW_BIO_HVO</t>
+  </si>
+  <si>
+    <t>RNW_BIO_DST_FT</t>
+  </si>
+  <si>
+    <t>ELC_CEN</t>
+  </si>
+  <si>
+    <t>ELC_DIS</t>
+  </si>
+  <si>
+    <t>PRI_OIL_GSL_kt</t>
+  </si>
+  <si>
+    <t>RNW_BIO_ETBE</t>
+  </si>
+  <si>
+    <t>RNW_BIO_ETH</t>
+  </si>
+  <si>
+    <t>PRI_OIL_LPG</t>
+  </si>
+  <si>
+    <t>PRI_GAS_NGA</t>
+  </si>
+  <si>
+    <t>SYN_CCUS_NGA</t>
+  </si>
+  <si>
+    <t>RNW_POT_BIO_GAS</t>
+  </si>
+  <si>
+    <t>HH2_BL</t>
+  </si>
+  <si>
+    <t>PRI_GAS_LNG</t>
+  </si>
+  <si>
+    <t>HH2_WE_CU</t>
+  </si>
+  <si>
+    <t>HH2_WE_DT</t>
+  </si>
+  <si>
+    <t>SYN_MTH</t>
+  </si>
+  <si>
     <t>output_comm</t>
   </si>
   <si>
-    <t>TRA_FT_COA</t>
-  </si>
-  <si>
-    <t>TRA_FT_AVG</t>
-  </si>
-  <si>
-    <t>TRA_FT_DST</t>
-  </si>
-  <si>
-    <t>TRA_FT_ELC</t>
-  </si>
-  <si>
-    <t>TRA_FT_GSL</t>
-  </si>
-  <si>
-    <t>TRA_FT_HFO</t>
-  </si>
-  <si>
-    <t>TRA_FT_JTK</t>
-  </si>
-  <si>
-    <t>TRA_FT_LPG</t>
-  </si>
-  <si>
-    <t>TRA_FT_NGA</t>
-  </si>
-  <si>
-    <t>TRA_FT_LNG</t>
-  </si>
-  <si>
-    <t>TRA_FT_ETH</t>
-  </si>
-  <si>
-    <t>TRA_FT_AMM_ELCSYS_CU</t>
-  </si>
-  <si>
-    <t>TRA_FT_MTH</t>
-  </si>
-  <si>
     <t>HH2_DEL_TRA_LH2_C_1_NEW</t>
   </si>
   <si>
     <t>HH2_DEL_TRA_GH2_C_4_NEW</t>
   </si>
   <si>
-    <t>HH2_DEL_TRA_GH2_C_5_NEW</t>
-  </si>
-  <si>
-    <t>HH2_DEL_TRA_LH2_D_1_NEW</t>
-  </si>
-  <si>
     <t>TRA_COA</t>
   </si>
   <si>
@@ -120,9 +177,6 @@
   </si>
   <si>
     <t>TRA_HFO</t>
-  </si>
-  <si>
-    <t>TRA_JTK</t>
   </si>
   <si>
     <t>TRA_LPG</t>
@@ -504,13 +558,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:L1"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:12">
+    <row r="1" spans="1:12">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -543,6 +597,994 @@
       </c>
       <c r="L1" s="1" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2">
+        <v>0.582</v>
+      </c>
+      <c r="E2">
+        <v>0.439</v>
+      </c>
+      <c r="F2">
+        <v>0.369</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0.1460600635005932</v>
+      </c>
+      <c r="H3">
+        <v>0.07303003175029658</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4">
+        <v>3.548458638278998</v>
+      </c>
+      <c r="E4">
+        <v>2.838766910623198</v>
+      </c>
+      <c r="F4">
+        <v>2.129075182967398</v>
+      </c>
+      <c r="G4">
+        <v>1.419383455311599</v>
+      </c>
+      <c r="H4">
+        <v>0.7096917276557995</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5">
+        <v>199665.9831971876</v>
+      </c>
+      <c r="E5">
+        <v>208121.5670326729</v>
+      </c>
+      <c r="F5">
+        <v>184028.0082534129</v>
+      </c>
+      <c r="G5">
+        <v>225761.0857577356</v>
+      </c>
+      <c r="H5">
+        <v>186974.2500932919</v>
+      </c>
+      <c r="I5">
+        <v>114649.5822712708</v>
+      </c>
+      <c r="J5">
+        <v>21134.15917895039</v>
+      </c>
+      <c r="K5">
+        <v>10587.74740732306</v>
+      </c>
+      <c r="L5">
+        <v>8340.810918444538</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6">
+        <v>6787.159667516534</v>
+      </c>
+      <c r="E6">
+        <v>11277.51262509778</v>
+      </c>
+      <c r="F6">
+        <v>12526.67045773545</v>
+      </c>
+      <c r="G6">
+        <v>13137.16725752518</v>
+      </c>
+      <c r="H6">
+        <v>23051.12395520314</v>
+      </c>
+      <c r="I6">
+        <v>28401.07347768795</v>
+      </c>
+      <c r="J6">
+        <v>3067.861816299249</v>
+      </c>
+      <c r="K6">
+        <v>2475.057835478116</v>
+      </c>
+      <c r="L6">
+        <v>388.8370850760846</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>58992.55144734716</v>
+      </c>
+      <c r="K7">
+        <v>51761.76934204461</v>
+      </c>
+      <c r="L7">
+        <v>4231.588165682198</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>17006.0365338585</v>
+      </c>
+      <c r="G8">
+        <v>18361.78100303936</v>
+      </c>
+      <c r="H8">
+        <v>19638.65461218345</v>
+      </c>
+      <c r="I8">
+        <v>19466.33258359015</v>
+      </c>
+      <c r="J8">
+        <v>19067.48810071151</v>
+      </c>
+      <c r="K8">
+        <v>17677.35326442478</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9">
+        <v>242.1597886419349</v>
+      </c>
+      <c r="E9">
+        <v>242.1199363221267</v>
+      </c>
+      <c r="F9">
+        <v>232.161583327048</v>
+      </c>
+      <c r="G9">
+        <v>264.1725169490221</v>
+      </c>
+      <c r="H9">
+        <v>650.8156710495325</v>
+      </c>
+      <c r="I9">
+        <v>991.7554874988263</v>
+      </c>
+      <c r="J9">
+        <v>1063.33129230369</v>
+      </c>
+      <c r="K9">
+        <v>1381.768157471506</v>
+      </c>
+      <c r="L9">
+        <v>1651.044655985398</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10">
+        <v>1.366521585484395</v>
+      </c>
+      <c r="E10">
+        <v>8.076904107402809</v>
+      </c>
+      <c r="F10">
+        <v>11.33003728682171</v>
+      </c>
+      <c r="G10">
+        <v>63.45194451960064</v>
+      </c>
+      <c r="H10">
+        <v>166.9585837490222</v>
+      </c>
+      <c r="I10">
+        <v>441.3944300310362</v>
+      </c>
+      <c r="J10">
+        <v>635.8333942735426</v>
+      </c>
+      <c r="K10">
+        <v>1094.518863086748</v>
+      </c>
+      <c r="L10">
+        <v>1525.705130118729</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11">
+        <v>77241.74789251573</v>
+      </c>
+      <c r="E11">
+        <v>63090.53403311125</v>
+      </c>
+      <c r="F11">
+        <v>55757.91715482286</v>
+      </c>
+      <c r="G11">
+        <v>44027.49799429774</v>
+      </c>
+      <c r="H11">
+        <v>27774.88213719858</v>
+      </c>
+      <c r="I11">
+        <v>4879.996985156938</v>
+      </c>
+      <c r="J11">
+        <v>2982.985460231999</v>
+      </c>
+      <c r="K11">
+        <v>75.38590367211781</v>
+      </c>
+      <c r="L11">
+        <v>7073.080162378212</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12">
+        <v>13910.83611334406</v>
+      </c>
+      <c r="E12">
+        <v>12053.60209256926</v>
+      </c>
+      <c r="F12">
+        <v>10660.63321702273</v>
+      </c>
+      <c r="G12">
+        <v>8417.836094507244</v>
+      </c>
+      <c r="H12">
+        <v>5310.417716797718</v>
+      </c>
+      <c r="I12">
+        <v>933.0308701180561</v>
+      </c>
+      <c r="J12">
+        <v>570.331811264483</v>
+      </c>
+      <c r="K12">
+        <v>14.41340548196466</v>
+      </c>
+      <c r="L12">
+        <v>1352.337339221998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13">
+        <v>366.074634561686</v>
+      </c>
+      <c r="E13">
+        <v>4155.877641222517</v>
+      </c>
+      <c r="F13">
+        <v>3717.19447698819</v>
+      </c>
+      <c r="G13">
+        <v>2935.166532953182</v>
+      </c>
+      <c r="H13">
+        <v>1851.658809146573</v>
+      </c>
+      <c r="I13">
+        <v>325.3331323437959</v>
+      </c>
+      <c r="J13">
+        <v>198.8656973488</v>
+      </c>
+      <c r="K13">
+        <v>5.02572691147452</v>
+      </c>
+      <c r="L13">
+        <v>471.5386774918809</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14">
+        <v>2828.845478712951</v>
+      </c>
+      <c r="E14">
+        <v>3431.79528313746</v>
+      </c>
+      <c r="F14">
+        <v>5038.530854660924</v>
+      </c>
+      <c r="G14">
+        <v>8389.62673346625</v>
+      </c>
+      <c r="H14">
+        <v>3114.830452806797</v>
+      </c>
+      <c r="I14">
+        <v>353.8280229550123</v>
+      </c>
+      <c r="J14">
+        <v>77.58762007899041</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>283.9471558182777</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>2322.522793957983</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>1974.173888676534</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>8707.712778427182</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16">
+        <v>143.5350814331654</v>
+      </c>
+      <c r="E16">
+        <v>64.06707444015838</v>
+      </c>
+      <c r="F16">
+        <v>8.698905109489051</v>
+      </c>
+      <c r="G16">
+        <v>8.698905109489051</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17">
+        <v>9.862565402026725</v>
+      </c>
+      <c r="E17">
+        <v>8.629744726773382</v>
+      </c>
+      <c r="F17">
+        <v>125.7548989382516</v>
+      </c>
+      <c r="G17">
+        <v>712.1125194525315</v>
+      </c>
+      <c r="H17">
+        <v>1186.129788582491</v>
+      </c>
+      <c r="I17">
+        <v>2484.988150602044</v>
+      </c>
+      <c r="J17">
+        <v>2868.372001947508</v>
+      </c>
+      <c r="K17">
+        <v>156.187932628838</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>981.906292303409</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19">
+        <v>0.5190823895803539</v>
+      </c>
+      <c r="E19">
+        <v>1.232820675253341</v>
+      </c>
+      <c r="F19">
+        <v>31.83668327550674</v>
+      </c>
+      <c r="G19">
+        <v>366.1246886645409</v>
+      </c>
+      <c r="H19">
+        <v>1092.487963168083</v>
+      </c>
+      <c r="I19">
+        <v>1202.24550651637</v>
+      </c>
+      <c r="J19">
+        <v>1904.764409953347</v>
+      </c>
+      <c r="K19">
+        <v>1657.504591163179</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>1.591834163775336</v>
+      </c>
+      <c r="G20">
+        <v>20.13685787654974</v>
+      </c>
+      <c r="H20">
+        <v>62.42788360960478</v>
+      </c>
+      <c r="I20">
+        <v>169.3470447976827</v>
+      </c>
+      <c r="J20">
+        <v>216.2047852080527</v>
+      </c>
+      <c r="K20">
+        <v>98.81277370395873</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0.9899090011670065</v>
+      </c>
+      <c r="H21">
+        <v>6.152637391702759</v>
+      </c>
+      <c r="I21">
+        <v>38.31239935269516</v>
+      </c>
+      <c r="J21">
+        <v>225.4351405628443</v>
+      </c>
+      <c r="K21">
+        <v>501.6846242060892</v>
+      </c>
+      <c r="L21">
+        <v>827.9899063660972</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22">
+        <v>4.277305825242719</v>
+      </c>
+      <c r="E22">
+        <v>2.138652912621359</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0.172882497426718</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0.0211259765142098</v>
+      </c>
+      <c r="I23">
+        <v>0.0211259765142098</v>
+      </c>
+      <c r="J23">
+        <v>0.4179430838190962</v>
+      </c>
+      <c r="K23">
+        <v>0.3968171073048865</v>
+      </c>
+      <c r="L23">
+        <v>0.397871558203522</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0.170928355433152</v>
+      </c>
+      <c r="I24">
+        <v>0.170928355433152</v>
+      </c>
+      <c r="J24">
+        <v>3.381539496354506</v>
+      </c>
+      <c r="K24">
+        <v>3.210611140921354</v>
+      </c>
+      <c r="L24">
+        <v>3.219142607283042</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>4.680966533537863</v>
+      </c>
+      <c r="J25">
+        <v>27.29323730528169</v>
+      </c>
+      <c r="K25">
+        <v>4.680966533537863</v>
+      </c>
+      <c r="L25">
+        <v>128.2645118870454</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>37.87327468044271</v>
+      </c>
+      <c r="J26">
+        <v>220.8271018336428</v>
+      </c>
+      <c r="K26">
+        <v>37.87327468044271</v>
+      </c>
+      <c r="L26">
+        <v>1037.776505267912</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0.9899090011670064</v>
+      </c>
+      <c r="J27">
+        <v>6.152637391702759</v>
+      </c>
+      <c r="K27">
+        <v>38.31239935269517</v>
+      </c>
+      <c r="L27">
+        <v>225.4351405628443</v>
       </c>
     </row>
   </sheetData>
@@ -552,7 +1594,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -563,7 +1605,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -598,25 +1640,25 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="D2">
-        <v>0.4785746154511807</v>
+        <v>0.582</v>
       </c>
       <c r="E2">
-        <v>0.2392873077255906</v>
+        <v>0.439</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>0.369</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>0.1460600635005932</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>0.07303003175029658</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -636,25 +1678,25 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="D3">
         <v>3.548458638278998</v>
       </c>
       <c r="E3">
-        <v>1.774229319139499</v>
+        <v>2.838766910623198</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>2.129075182967398</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>1.419383455311599</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>0.7096917276557995</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -674,37 +1716,37 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="D4">
-        <v>9906.174086013527</v>
+        <v>8836.762185177176</v>
       </c>
       <c r="E4">
-        <v>10551.75712524956</v>
+        <v>9366.495349533556</v>
       </c>
       <c r="F4">
-        <v>9748.742825153013</v>
+        <v>9124.956769322736</v>
       </c>
       <c r="G4">
-        <v>6242.727025054065</v>
+        <v>11001.72024024479</v>
       </c>
       <c r="H4">
-        <v>1922.030378255188</v>
+        <v>9756.885143290139</v>
       </c>
       <c r="I4">
-        <v>1922.030378255188</v>
+        <v>6837.290390017067</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>4456.921472012521</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>3602.171673112233</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>559.2317209309471</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -712,37 +1754,37 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="D5">
-        <v>10.94109791489978</v>
+        <v>225.296</v>
       </c>
       <c r="E5">
-        <v>43.18559082926281</v>
+        <v>231.634</v>
       </c>
       <c r="F5">
-        <v>158.2917422657747</v>
+        <v>225.513</v>
       </c>
       <c r="G5">
-        <v>1185.050375144579</v>
+        <v>304.638925471466</v>
       </c>
       <c r="H5">
-        <v>3623.846275378929</v>
+        <v>760.615150282389</v>
       </c>
       <c r="I5">
-        <v>3717.5891301546</v>
+        <v>1336.698534465898</v>
       </c>
       <c r="J5">
-        <v>4588.625001530096</v>
+        <v>1587.623169940778</v>
       </c>
       <c r="K5">
-        <v>3907.308115487804</v>
+        <v>2317.928465593553</v>
       </c>
       <c r="L5">
-        <v>2999.434872309661</v>
+        <v>2976.636180399286</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -750,37 +1792,37 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="D6">
-        <v>4569.785334781945</v>
+        <v>3832.069274591728</v>
       </c>
       <c r="E6">
-        <v>4345.080211090862</v>
+        <v>3259.031335069285</v>
       </c>
       <c r="F6">
-        <v>3403.989046900169</v>
+        <v>2881.737484348883</v>
       </c>
       <c r="G6">
-        <v>3458.474171064247</v>
+        <v>2275.4740095468</v>
       </c>
       <c r="H6">
-        <v>3.549761135429597E-05</v>
+        <v>1435.489757551214</v>
       </c>
       <c r="I6">
-        <v>59.83305705362738</v>
+        <v>252.2129762592809</v>
       </c>
       <c r="J6">
-        <v>1.288491591290545</v>
+        <v>154.1696938239149</v>
       </c>
       <c r="K6">
-        <v>4.239502152556725</v>
+        <v>3.896171081861606</v>
       </c>
       <c r="L6">
-        <v>8.377272150998138</v>
+        <v>365.5581354865358</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -788,37 +1830,37 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="D7">
-        <v>1067.265389572699</v>
+        <v>1626.815516109571</v>
       </c>
       <c r="E7">
-        <v>784.8292822628329</v>
+        <v>1973.560541475645</v>
       </c>
       <c r="F7">
-        <v>173.9653327146419</v>
+        <v>2035.489687669987</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>595.7887163855584</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>191.6843829439324</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>19.15619967634759</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>112.7175702814221</v>
       </c>
       <c r="K7">
         <v>0</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>413.9949531830488</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -826,37 +1868,37 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="D8">
-        <v>2045.858518334246</v>
+        <v>143.5350814331654</v>
       </c>
       <c r="E8">
-        <v>2092.117817980853</v>
+        <v>64.06707444015838</v>
       </c>
       <c r="F8">
-        <v>2037.398091741601</v>
+        <v>8.698905109489051</v>
       </c>
       <c r="G8">
-        <v>2217.782930268329</v>
+        <v>8.698905109489051</v>
       </c>
       <c r="H8">
-        <v>2295.122194303294</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <v>2362.965504566188</v>
+        <v>0</v>
       </c>
       <c r="J8">
-        <v>2419.566657104332</v>
+        <v>0</v>
       </c>
       <c r="K8">
-        <v>2470.031173329205</v>
+        <v>0</v>
       </c>
       <c r="L8">
-        <v>2513.127137123704</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -864,34 +1906,34 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="D9">
-        <v>160.7082417804549</v>
+        <v>10.29859460927422</v>
       </c>
       <c r="E9">
-        <v>254.216198788791</v>
+        <v>9.783664878810509</v>
       </c>
       <c r="F9">
-        <v>133.0395129746052</v>
+        <v>158.081</v>
       </c>
       <c r="G9">
-        <v>127.6656618035408</v>
+        <v>1091.370285878537</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>2326.768187769685</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>4810.705835579765</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>4960.750949516496</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>1901.955968873742</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -902,37 +1944,37 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="D10">
-        <v>657.1562232904943</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>691.2194767207457</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>688.8136422738996</v>
+        <v>0</v>
       </c>
       <c r="G10">
-        <v>426.3543854557249</v>
+        <v>0.9899090011670065</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>6.152637391702759</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>38.31239935269516</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>225.4351405628443</v>
       </c>
       <c r="K10">
-        <v>0</v>
+        <v>501.6846242060892</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>827.9899063660972</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -940,37 +1982,37 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="D11">
-        <v>1037.654216802169</v>
+        <v>4.277305825242719</v>
       </c>
       <c r="E11">
-        <v>1110.953890879406</v>
+        <v>2.138652912621359</v>
       </c>
       <c r="F11">
-        <v>1806.774844121201</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>3608.854877352575</v>
+        <v>0</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11">
-        <v>2625.662835502857</v>
+        <v>0</v>
       </c>
       <c r="J11">
-        <v>2667.915700913318</v>
+        <v>0</v>
       </c>
       <c r="K11">
-        <v>2675.564264694383</v>
+        <v>0</v>
       </c>
       <c r="L11">
-        <v>2253.654068883277</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -978,37 +2020,37 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="D12">
-        <v>70.3613756251349</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>68.11053342412207</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>0.07969883131371704</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>0.08853704702773382</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>0.08853704702773381</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>1.751561469460031</v>
       </c>
       <c r="K12">
-        <v>0</v>
+        <v>1.663024422432297</v>
       </c>
       <c r="L12">
-        <v>0</v>
+        <v>1.667443530289306</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1016,10 +2058,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1037,16 +2079,16 @@
         <v>0</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>19.61750519964504</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>114.3834763430442</v>
       </c>
       <c r="K13">
-        <v>0</v>
+        <v>19.61750519964504</v>
       </c>
       <c r="L13">
-        <v>139.480863074283</v>
+        <v>537.5449089084356</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1054,10 +2096,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -1072,19 +2114,19 @@
         <v>0</v>
       </c>
       <c r="H14">
-        <v>2566.432223054782</v>
+        <v>0</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>0.9899090011670064</v>
       </c>
       <c r="J14">
-        <v>0</v>
+        <v>6.152637391702759</v>
       </c>
       <c r="K14">
-        <v>0</v>
+        <v>38.31239935269517</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>225.4351405628443</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1092,10 +2134,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -1110,19 +2152,19 @@
         <v>0</v>
       </c>
       <c r="H15">
-        <v>0.009684439608269856</v>
+        <v>0.008705114254624611</v>
       </c>
       <c r="I15">
-        <v>0.06021037359448662</v>
+        <v>0.9466312404074463</v>
       </c>
       <c r="J15">
-        <v>6.267581490441001</v>
+        <v>5.897427223869264</v>
       </c>
       <c r="K15">
-        <v>40.80379887348116</v>
+        <v>36.72396407752533</v>
       </c>
       <c r="L15">
-        <v>240.8434761557383</v>
+        <v>216.1033327415356</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1130,10 +2172,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1148,95 +2190,19 @@
         <v>0</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>2.656993306345552</v>
       </c>
       <c r="I16">
-        <v>0.0166744069084333</v>
+        <v>59.79719436878673</v>
       </c>
       <c r="J16">
-        <v>394.1928314977513</v>
+        <v>657.8983717263446</v>
       </c>
       <c r="K16">
-        <v>1281.517564630858</v>
+        <v>1178.330451602167</v>
       </c>
       <c r="L16">
-        <v>2409.326263825856</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
-      <c r="A17" s="1">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17">
-        <v>17.28194042056948</v>
-      </c>
-      <c r="K17">
-        <v>56.18344229070566</v>
-      </c>
-      <c r="L17">
-        <v>105.6280825476888</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
-      <c r="A18" s="1">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <v>0.2747791467625491</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
+        <v>1332.696718292549</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor updates heat generation
</commit_message>
<xml_diff>
--- a/TEMOA_Europe_Results/_1_Transport_fueltechs.xlsx
+++ b/TEMOA_Europe_Results/_1_Transport_fueltechs.xlsx
@@ -89,7 +89,7 @@
     <t>PRI_COA_HCO</t>
   </si>
   <si>
-    <t>PRI_OIL_AVG</t>
+    <t>PRI_COA_BCO</t>
   </si>
   <si>
     <t>PRI_OIL_JTG</t>
@@ -128,9 +128,6 @@
     <t>PRI_GAS_NGA</t>
   </si>
   <si>
-    <t>SYN_CCUS_NGA</t>
-  </si>
-  <si>
     <t>RNW_POT_BIO_GAS</t>
   </si>
   <si>
@@ -156,6 +153,9 @@
   </si>
   <si>
     <t>HH2_DEL_TRA_LH2_C_1_NEW</t>
+  </si>
+  <si>
+    <t>HH2_DEL_TRA_LH2_C_2_NEW</t>
   </si>
   <si>
     <t>HH2_DEL_TRA_GH2_C_4_NEW</t>
@@ -558,7 +558,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -610,19 +610,19 @@
         <v>23</v>
       </c>
       <c r="D2">
-        <v>0.5819999999999999</v>
+        <v>0.582</v>
       </c>
       <c r="E2">
-        <v>0.439</v>
+        <v>0.334</v>
       </c>
       <c r="F2">
-        <v>0.3689999999999999</v>
+        <v>0.264</v>
       </c>
       <c r="G2">
         <v>0.1460600635005933</v>
       </c>
       <c r="H2">
-        <v>0.07303003175029658</v>
+        <v>0</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -642,7 +642,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
@@ -651,16 +651,16 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>2.838766910623198</v>
+        <v>0.105</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>0.105</v>
       </c>
       <c r="G3">
-        <v>1.419383455311599</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>0.0730300317502966</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -689,13 +689,13 @@
         <v>3.548458638278998</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>2.838766910623198</v>
       </c>
       <c r="F4">
         <v>2.129075182967398</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>1.419383455311599</v>
       </c>
       <c r="H4">
         <v>0.7096917276557995</v>
@@ -724,31 +724,31 @@
         <v>26</v>
       </c>
       <c r="D5">
-        <v>194899.0679140865</v>
+        <v>198982.8156135253</v>
       </c>
       <c r="E5">
-        <v>204056.018223721</v>
+        <v>204242.1749637213</v>
       </c>
       <c r="F5">
-        <v>176268.4994535297</v>
+        <v>176809.0812363035</v>
       </c>
       <c r="G5">
-        <v>223117.3217721705</v>
+        <v>229372.870751458</v>
       </c>
       <c r="H5">
-        <v>185490.1658012915</v>
+        <v>191828.4347297169</v>
       </c>
       <c r="I5">
-        <v>113829.5854452836</v>
+        <v>118852.1017272293</v>
       </c>
       <c r="J5">
-        <v>21103.11006417502</v>
+        <v>20160.00890140725</v>
       </c>
       <c r="K5">
-        <v>10579.69488503417</v>
+        <v>12337.94626304703</v>
       </c>
       <c r="L5">
-        <v>895.3847315911765</v>
+        <v>1565.086332553496</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -762,31 +762,31 @@
         <v>27</v>
       </c>
       <c r="D6">
-        <v>11241</v>
+        <v>7418.568219084142</v>
       </c>
       <c r="E6">
-        <v>14709.30790823524</v>
+        <v>14709.30790823598</v>
       </c>
       <c r="F6">
-        <v>20224.42620887413</v>
+        <v>19335.4262232156</v>
       </c>
       <c r="G6">
-        <v>21526.79399099141</v>
+        <v>21526.79399099144</v>
       </c>
       <c r="H6">
-        <v>26165.95440800994</v>
+        <v>26165.95440800993</v>
       </c>
       <c r="I6">
-        <v>28754.56429676541</v>
+        <v>28754.99863628495</v>
       </c>
       <c r="J6">
-        <v>3063.354686735083</v>
+        <v>2926.452905042988</v>
       </c>
       <c r="K6">
-        <v>2473.175427670324</v>
+        <v>2884.195230322684</v>
       </c>
       <c r="L6">
-        <v>383.7363135390759</v>
+        <v>939.0517995320976</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -818,13 +818,13 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>60975.92051152731</v>
+        <v>60102.8394409051</v>
       </c>
       <c r="K7">
-        <v>53807.00781719436</v>
+        <v>67948.70543292888</v>
       </c>
       <c r="L7">
-        <v>11512.08940617228</v>
+        <v>20003.50253104742</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -856,13 +856,13 @@
         <v>19466.33258359015</v>
       </c>
       <c r="J8">
-        <v>16969.43762873199</v>
+        <v>14359.12892074427</v>
       </c>
       <c r="K8">
-        <v>15579.30279244524</v>
+        <v>12968.99408445752</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>8794.085987936915</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -876,7 +876,7 @@
         <v>30</v>
       </c>
       <c r="D9">
-        <v>240.0905927553906</v>
+        <v>241.4490648374262</v>
       </c>
       <c r="E9">
         <v>242.1199363221268</v>
@@ -885,22 +885,22 @@
         <v>232.161583327048</v>
       </c>
       <c r="G9">
-        <v>289.8134900953373</v>
+        <v>262.7649967022483</v>
       </c>
       <c r="H9">
-        <v>662.6696852132887</v>
+        <v>611.5562900097099</v>
       </c>
       <c r="I9">
-        <v>1034.122567332392</v>
+        <v>1007.650494806335</v>
       </c>
       <c r="J9">
-        <v>1056.452307088769</v>
+        <v>1088.739943476629</v>
       </c>
       <c r="K9">
-        <v>1382.560292308656</v>
+        <v>1377.531199642253</v>
       </c>
       <c r="L9">
-        <v>1627.976364541361</v>
+        <v>1696.504881919234</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -914,31 +914,31 @@
         <v>31</v>
       </c>
       <c r="D10">
-        <v>3.381264948698568</v>
+        <v>2.058542131979698</v>
       </c>
       <c r="E10">
-        <v>8.076904107402809</v>
+        <v>8.076904107402811</v>
       </c>
       <c r="F10">
         <v>11.33003728682171</v>
       </c>
       <c r="G10">
-        <v>38.48573382450374</v>
+        <v>39.0685286250268</v>
       </c>
       <c r="H10">
-        <v>155.4165173264175</v>
+        <v>168.6577354556589</v>
       </c>
       <c r="I10">
-        <v>400.1422733509855</v>
+        <v>425.6095355729003</v>
       </c>
       <c r="J10">
-        <v>642.5918959296905</v>
+        <v>625.8261300505758</v>
       </c>
       <c r="K10">
-        <v>1095.146324731946</v>
+        <v>1090.700880055701</v>
       </c>
       <c r="L10">
-        <v>1577.062487478767</v>
+        <v>1696.504881919234</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -952,31 +952,31 @@
         <v>32</v>
       </c>
       <c r="D11">
-        <v>78611.69093903071</v>
+        <v>75161.48772542756</v>
       </c>
       <c r="E11">
-        <v>63091.81360350939</v>
+        <v>63058.06832603392</v>
       </c>
       <c r="F11">
         <v>55542.63651569869</v>
       </c>
       <c r="G11">
-        <v>43918.95812426761</v>
+        <v>43918.95812426758</v>
       </c>
       <c r="H11">
-        <v>27559.63951260178</v>
+        <v>27559.44845161116</v>
       </c>
       <c r="I11">
-        <v>4880.130574026493</v>
+        <v>4877.669203698396</v>
       </c>
       <c r="J11">
-        <v>2982.987799192995</v>
+        <v>2981.470868606867</v>
       </c>
       <c r="K11">
-        <v>75.25129154726832</v>
+        <v>76.21218936394932</v>
       </c>
       <c r="L11">
-        <v>6100.108866813765</v>
+        <v>94.03398386871736</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -990,31 +990,31 @@
         <v>33</v>
       </c>
       <c r="D12">
-        <v>12122.5341144703</v>
+        <v>14059.61842364205</v>
       </c>
       <c r="E12">
-        <v>12053.49239448662</v>
+        <v>12056.38539063793</v>
       </c>
       <c r="F12">
         <v>10619.47264199522</v>
       </c>
       <c r="G12">
-        <v>8397.083817470033</v>
+        <v>8397.083817470029</v>
       </c>
       <c r="H12">
-        <v>5269.264409956568</v>
+        <v>5269.227880056473</v>
       </c>
       <c r="I12">
-        <v>933.05641163777</v>
+        <v>932.5858100152909</v>
       </c>
       <c r="J12">
-        <v>570.332258462057</v>
+        <v>570.0422289663444</v>
       </c>
       <c r="K12">
-        <v>14.38766832098715</v>
+        <v>14.57138714883057</v>
       </c>
       <c r="L12">
-        <v>1166.310122963135</v>
+        <v>17.9788245887359</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1028,10 +1028,10 @@
         <v>34</v>
       </c>
       <c r="D13">
-        <v>364.3944781265101</v>
+        <v>3276.383480154389</v>
       </c>
       <c r="E13">
-        <v>4153.986070994922</v>
+        <v>4203.871221735594</v>
       </c>
       <c r="F13">
         <v>3702.842434379913</v>
@@ -1040,19 +1040,19 @@
         <v>2927.930541617839</v>
       </c>
       <c r="H13">
-        <v>1837.309300840119</v>
+        <v>1837.296563440744</v>
       </c>
       <c r="I13">
-        <v>325.3420382684329</v>
+        <v>325.1779469132264</v>
       </c>
       <c r="J13">
-        <v>198.865853279533</v>
+        <v>198.7647245737911</v>
       </c>
       <c r="K13">
-        <v>5.016752769817888</v>
+        <v>5.080812624263288</v>
       </c>
       <c r="L13">
-        <v>406.6739244542509</v>
+        <v>6.268932257914494</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1066,16 +1066,16 @@
         <v>35</v>
       </c>
       <c r="D14">
-        <v>199.7801343600287</v>
+        <v>179.5189976813809</v>
       </c>
       <c r="E14">
-        <v>120.3121273670217</v>
+        <v>100.0509906883739</v>
       </c>
       <c r="F14">
-        <v>64.94395803635236</v>
+        <v>37.3515383330611</v>
       </c>
       <c r="G14">
-        <v>64.94395803635236</v>
+        <v>44.68282135770457</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -1104,28 +1104,28 @@
         <v>36</v>
       </c>
       <c r="D15">
-        <v>9.86256540202673</v>
+        <v>9.862565402026727</v>
       </c>
       <c r="E15">
-        <v>8.629744726773382</v>
+        <v>8.629744726773383</v>
       </c>
       <c r="F15">
         <v>125.7548989382516</v>
       </c>
       <c r="G15">
-        <v>686.4534373031286</v>
+        <v>544.6918750569678</v>
       </c>
       <c r="H15">
-        <v>1165.346806319244</v>
+        <v>1064.423192185728</v>
       </c>
       <c r="I15">
-        <v>2522.027923223919</v>
+        <v>3303.532621003183</v>
       </c>
       <c r="J15">
-        <v>2865.538799217046</v>
+        <v>3118.691579497728</v>
       </c>
       <c r="K15">
-        <v>156.7452078287533</v>
+        <v>146.2491829300208</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -1142,28 +1142,28 @@
         <v>37</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>0.519082389580354</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>1.23282067525334</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>31.83668327550674</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>280.0472365331455</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>980.3897822763289</v>
       </c>
       <c r="I16">
-        <v>976.242495078908</v>
+        <v>1225.303906516373</v>
       </c>
       <c r="J16">
-        <v>0</v>
+        <v>1915.011843415477</v>
       </c>
       <c r="K16">
-        <v>0</v>
+        <v>1552.032145379815</v>
       </c>
       <c r="L16">
         <v>0</v>
@@ -1180,28 +1180,28 @@
         <v>38</v>
       </c>
       <c r="D17">
-        <v>0.5190823895803541</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>1.232820675253341</v>
+        <v>0</v>
       </c>
       <c r="F17">
-        <v>31.83668327550673</v>
+        <v>1.591834163775336</v>
       </c>
       <c r="G17">
-        <v>352.9323585106061</v>
+        <v>15.402598009323</v>
       </c>
       <c r="H17">
-        <v>1073.345742662462</v>
+        <v>56.02227327293309</v>
       </c>
       <c r="I17">
-        <v>1202.245506516373</v>
+        <v>164.2583196509684</v>
       </c>
       <c r="J17">
-        <v>1912.511992911922</v>
+        <v>228.0074721180197</v>
       </c>
       <c r="K17">
-        <v>1663.41853206024</v>
+        <v>92.52499328225839</v>
       </c>
       <c r="L17">
         <v>0</v>
@@ -1212,7 +1212,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C18" t="s">
         <v>39</v>
@@ -1224,22 +1224,22 @@
         <v>0</v>
       </c>
       <c r="F18">
-        <v>1.591834163775336</v>
+        <v>0</v>
       </c>
       <c r="G18">
-        <v>19.41127971808334</v>
+        <v>0.9899090011670063</v>
       </c>
       <c r="H18">
-        <v>61.33404243785498</v>
+        <v>6.152637391702759</v>
       </c>
       <c r="I18">
-        <v>170.4850335426649</v>
+        <v>38.31239935269515</v>
       </c>
       <c r="J18">
-        <v>216.4273877967826</v>
+        <v>225.4351405628443</v>
       </c>
       <c r="K18">
-        <v>99.16533556512969</v>
+        <v>0</v>
       </c>
       <c r="L18">
         <v>0</v>
@@ -1250,37 +1250,37 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>4.277305825242719</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>2.138652912621359</v>
       </c>
       <c r="F19">
         <v>0</v>
       </c>
       <c r="G19">
-        <v>0.9899090011670065</v>
+        <v>0</v>
       </c>
       <c r="H19">
-        <v>6.152637391702759</v>
+        <v>0</v>
       </c>
       <c r="I19">
-        <v>38.31239935269515</v>
+        <v>0</v>
       </c>
       <c r="J19">
-        <v>225.4351405628443</v>
+        <v>0</v>
       </c>
       <c r="K19">
-        <v>497.7546650742136</v>
+        <v>0</v>
       </c>
       <c r="L19">
-        <v>827.9899063660972</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1288,16 +1288,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D20">
-        <v>4.277305825242719</v>
+        <v>0</v>
       </c>
       <c r="E20">
-        <v>2.138652912621359</v>
+        <v>0</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -1312,13 +1312,13 @@
         <v>0</v>
       </c>
       <c r="J20">
-        <v>0</v>
+        <v>23.00908787904872</v>
       </c>
       <c r="K20">
-        <v>0</v>
+        <v>0.3947082055076144</v>
       </c>
       <c r="L20">
-        <v>0</v>
+        <v>23.00908787904872</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1329,7 +1329,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -1344,19 +1344,19 @@
         <v>0</v>
       </c>
       <c r="H21">
-        <v>0.00210890179727082</v>
+        <v>0</v>
       </c>
       <c r="I21">
-        <v>0.00210890179727082</v>
+        <v>0</v>
       </c>
       <c r="J21">
-        <v>17.93552204180051</v>
+        <v>186.1644382941215</v>
       </c>
       <c r="K21">
-        <v>0.00210890179727082</v>
+        <v>3.193548208197972</v>
       </c>
       <c r="L21">
-        <v>118.9057421726655</v>
+        <v>186.1644382941215</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -1364,10 +1364,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -1376,25 +1376,25 @@
         <v>0</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>0.172882497426718</v>
       </c>
       <c r="G22">
         <v>0</v>
       </c>
       <c r="H22">
-        <v>0.017062932723373</v>
+        <v>0.0211259765142098</v>
       </c>
       <c r="I22">
-        <v>0.017062932723373</v>
+        <v>4.702092510052073</v>
       </c>
       <c r="J22">
-        <v>145.1146783382042</v>
+        <v>4.702092510052073</v>
       </c>
       <c r="K22">
-        <v>0.017062932723373</v>
+        <v>4.683075435335134</v>
       </c>
       <c r="L22">
-        <v>962.0555503061123</v>
+        <v>105.6532955662002</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -1405,7 +1405,7 @@
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -1414,25 +1414,25 @@
         <v>0</v>
       </c>
       <c r="F23">
-        <v>0.172882497426718</v>
+        <v>0</v>
       </c>
       <c r="G23">
         <v>0</v>
       </c>
       <c r="H23">
-        <v>0.01901707471693898</v>
+        <v>0.170928355433152</v>
       </c>
       <c r="I23">
-        <v>4.699983608254802</v>
+        <v>38.04420303587586</v>
       </c>
       <c r="J23">
-        <v>9.775658347300279</v>
+        <v>38.04420303587586</v>
       </c>
       <c r="K23">
-        <v>5.075674739045478</v>
+        <v>37.89033761316609</v>
       </c>
       <c r="L23">
-        <v>9.756641272583341</v>
+        <v>854.8312095810742</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -1440,7 +1440,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C24" t="s">
         <v>42</v>
@@ -1458,56 +1458,18 @@
         <v>0</v>
       </c>
       <c r="H24">
-        <v>0.153865422709779</v>
+        <v>0</v>
       </c>
       <c r="I24">
-        <v>38.02714010315249</v>
+        <v>0.9899090011670064</v>
       </c>
       <c r="J24">
-        <v>79.09396299179318</v>
+        <v>6.152637391702759</v>
       </c>
       <c r="K24">
-        <v>41.06682288864068</v>
+        <v>38.31239935269517</v>
       </c>
       <c r="L24">
-        <v>78.94009756908339</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
-      <c r="A25" s="1">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" t="s">
-        <v>43</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
-      <c r="H25">
-        <v>0</v>
-      </c>
-      <c r="I25">
-        <v>0.9899090011670064</v>
-      </c>
-      <c r="J25">
-        <v>6.152637391702759</v>
-      </c>
-      <c r="K25">
-        <v>38.31239935269515</v>
-      </c>
-      <c r="L25">
         <v>225.4351405628443</v>
       </c>
     </row>
@@ -1518,7 +1480,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1529,7 +1491,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -1570,7 +1532,7 @@
         <v>48</v>
       </c>
       <c r="D2">
-        <v>0.5819999999999999</v>
+        <v>0.582</v>
       </c>
       <c r="E2">
         <v>0.439</v>
@@ -1582,7 +1544,7 @@
         <v>0.1460600635005933</v>
       </c>
       <c r="H2">
-        <v>0.07303003175029658</v>
+        <v>0.0730300317502966</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1646,31 +1608,31 @@
         <v>50</v>
       </c>
       <c r="D4">
-        <v>8796.576920305717</v>
+        <v>8830.748095487703</v>
       </c>
       <c r="E4">
-        <v>9318.653176224707</v>
+        <v>9326.65791604474</v>
       </c>
       <c r="F4">
-        <v>9076.114853719891</v>
+        <v>9066.4668709098</v>
       </c>
       <c r="G4">
-        <v>11198.45457800375</v>
+        <v>11467.44318411311</v>
       </c>
       <c r="H4">
-        <v>9800.73607622987</v>
+        <v>10073.28164015216</v>
       </c>
       <c r="I4">
-        <v>6815.109686805478</v>
+        <v>7031.09395749137</v>
       </c>
       <c r="J4">
-        <v>4450.373614340133</v>
+        <v>4251.485748159676</v>
       </c>
       <c r="K4">
-        <v>3599.432037704413</v>
+        <v>4197.625691597962</v>
       </c>
       <c r="L4">
-        <v>559.2317209309468</v>
+        <v>1369.137523717798</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1693,22 +1655,22 @@
         <v>225.513</v>
       </c>
       <c r="G5">
-        <v>304.6389254714657</v>
+        <v>280.1727241433552</v>
       </c>
       <c r="H5">
-        <v>760.6151502823889</v>
+        <v>725.9144169418577</v>
       </c>
       <c r="I5">
-        <v>1336.698534465899</v>
+        <v>1336.405766490116</v>
       </c>
       <c r="J5">
-        <v>1587.680685190317</v>
+        <v>1601.619271263929</v>
       </c>
       <c r="K5">
-        <v>2319.257278880857</v>
+        <v>2310.382195722</v>
       </c>
       <c r="L5">
-        <v>3004.087500305588</v>
+        <v>3180.946653598565</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1722,7 +1684,7 @@
         <v>52</v>
       </c>
       <c r="D6">
-        <v>3826.552589408667</v>
+        <v>3826.552589408666</v>
       </c>
       <c r="E6">
         <v>3259.031335069285</v>
@@ -1731,22 +1693,22 @@
         <v>2870.611131015129</v>
       </c>
       <c r="G6">
-        <v>2269.86434139611</v>
+        <v>2269.864341396109</v>
       </c>
       <c r="H6">
-        <v>1424.365368922996</v>
+        <v>1424.355494314213</v>
       </c>
       <c r="I6">
-        <v>252.2198805353467</v>
+        <v>252.0926694862386</v>
       </c>
       <c r="J6">
-        <v>154.1698147084802</v>
+        <v>154.091415156376</v>
       </c>
       <c r="K6">
-        <v>3.889213920873158</v>
+        <v>3.938876020862829</v>
       </c>
       <c r="L6">
-        <v>315.2720416599295</v>
+        <v>4.859960162513031</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1754,22 +1716,22 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
         <v>53</v>
       </c>
       <c r="D7">
-        <v>1621.016639238097</v>
+        <v>1605.070043182009</v>
       </c>
       <c r="E7">
-        <v>1971.173192861564</v>
+        <v>1981.395153867322</v>
       </c>
       <c r="F7">
         <v>2035.489687669987</v>
       </c>
       <c r="G7">
-        <v>383.3687658878636</v>
+        <v>383.3687658878648</v>
       </c>
       <c r="H7">
         <v>191.6843829439324</v>
@@ -1784,7 +1746,7 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <v>413.994953183049</v>
+        <v>413.9949531830487</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1798,16 +1760,16 @@
         <v>54</v>
       </c>
       <c r="D8">
-        <v>199.7801343600287</v>
+        <v>179.5189976813809</v>
       </c>
       <c r="E8">
-        <v>120.3121273670217</v>
+        <v>100.0509906883739</v>
       </c>
       <c r="F8">
-        <v>64.94395803635236</v>
+        <v>37.3515383330611</v>
       </c>
       <c r="G8">
-        <v>64.94395803635236</v>
+        <v>44.68282135770457</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1836,28 +1798,28 @@
         <v>55</v>
       </c>
       <c r="D9">
-        <v>10.29859460927423</v>
+        <v>10.29859460927422</v>
       </c>
       <c r="E9">
-        <v>9.783664878810511</v>
+        <v>9.783664878810509</v>
       </c>
       <c r="F9">
         <v>158.081</v>
       </c>
       <c r="G9">
-        <v>1052.041982112067</v>
+        <v>834.7605630042511</v>
       </c>
       <c r="H9">
-        <v>2286.006234714114</v>
+        <v>2088.074685242437</v>
       </c>
       <c r="I9">
-        <v>4843.077545321553</v>
+        <v>4666.260300542878</v>
       </c>
       <c r="J9">
-        <v>4965.882860598841</v>
+        <v>5232.035090353493</v>
       </c>
       <c r="K9">
-        <v>1908.730264178597</v>
+        <v>1781.109308481964</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -1883,7 +1845,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>0.9899090011670065</v>
+        <v>0.9899090011670063</v>
       </c>
       <c r="H10">
         <v>6.152637391702759</v>
@@ -1895,10 +1857,10 @@
         <v>225.4351405628443</v>
       </c>
       <c r="K10">
-        <v>497.7546650742136</v>
+        <v>0</v>
       </c>
       <c r="L10">
-        <v>827.9899063660972</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1962,19 +1924,19 @@
         <v>0</v>
       </c>
       <c r="H12">
-        <v>0.008838215714016802</v>
+        <v>0</v>
       </c>
       <c r="I12">
-        <v>0.008838215714016802</v>
+        <v>0</v>
       </c>
       <c r="J12">
-        <v>75.16614237518213</v>
+        <v>96.42899556583146</v>
       </c>
       <c r="K12">
-        <v>0.008838215714016802</v>
+        <v>1.654186206718276</v>
       </c>
       <c r="L12">
-        <v>498.3231558327165</v>
+        <v>96.42899556583146</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -2000,19 +1962,19 @@
         <v>0</v>
       </c>
       <c r="H13">
-        <v>0.07969883131371701</v>
+        <v>0.08853704702773381</v>
       </c>
       <c r="I13">
-        <v>19.69720403095876</v>
+        <v>19.70604224667278</v>
       </c>
       <c r="J13">
-        <v>40.96889543732207</v>
+        <v>19.70604224667278</v>
       </c>
       <c r="K13">
-        <v>21.27169140636332</v>
+        <v>19.62634341535906</v>
       </c>
       <c r="L13">
-        <v>40.88919660600836</v>
+        <v>442.7833568728934</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -2047,7 +2009,7 @@
         <v>6.152637391702759</v>
       </c>
       <c r="K14">
-        <v>38.31239935269515</v>
+        <v>38.31239935269517</v>
       </c>
       <c r="L14">
         <v>225.4351405628443</v>
@@ -2058,7 +2020,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
         <v>60</v>
@@ -2076,19 +2038,19 @@
         <v>0</v>
       </c>
       <c r="H15">
-        <v>0.008705114254624592</v>
+        <v>0</v>
       </c>
       <c r="I15">
-        <v>0.9466312404074462</v>
+        <v>0.9379261261528213</v>
       </c>
       <c r="J15">
-        <v>5.897427223869263</v>
+        <v>5.88872210961464</v>
       </c>
       <c r="K15">
-        <v>36.72396407752534</v>
+        <v>36.71525896327071</v>
       </c>
       <c r="L15">
-        <v>216.1033327415356</v>
+        <v>216.1033327415355</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -2096,37 +2058,75 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0.00870511425462459</v>
+      </c>
+      <c r="I16">
+        <v>0.008705114254624557</v>
+      </c>
+      <c r="J16">
+        <v>0.008705114254624471</v>
+      </c>
+      <c r="K16">
+        <v>0.008705114254624592</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
         <v>47</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>61</v>
       </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>3.245230391497282</v>
-      </c>
-      <c r="I16">
-        <v>61.93521852382509</v>
-      </c>
-      <c r="J16">
-        <v>657.9358056467354</v>
-      </c>
-      <c r="K16">
-        <v>1176.176050749412</v>
-      </c>
-      <c r="L16">
-        <v>1332.720061711963</v>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>22.54219698339416</v>
+      </c>
+      <c r="J17">
+        <v>633.6580776784569</v>
+      </c>
+      <c r="K17">
+        <v>1191.55474771288</v>
+      </c>
+      <c r="L17">
+        <v>1339.118844065566</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to oil and gas import availability
</commit_message>
<xml_diff>
--- a/TEMOA_Europe_Results/_1_Transport_fueltechs.xlsx
+++ b/TEMOA_Europe_Results/_1_Transport_fueltechs.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="64">
   <si>
     <t>tech</t>
   </si>
@@ -65,6 +65,9 @@
     <t>TRA_FT_GSL</t>
   </si>
   <si>
+    <t>TRA_FT_HFO</t>
+  </si>
+  <si>
     <t>TRA_FT_LPG</t>
   </si>
   <si>
@@ -92,6 +95,9 @@
     <t>PRI_COA_BCO</t>
   </si>
   <si>
+    <t>PRI_OIL_AVG</t>
+  </si>
+  <si>
     <t>PRI_OIL_JTG</t>
   </si>
   <si>
@@ -122,6 +128,9 @@
     <t>RNW_BIO_ETH</t>
   </si>
   <si>
+    <t>PRI_OIL_HFO</t>
+  </si>
+  <si>
     <t>PRI_OIL_LPG</t>
   </si>
   <si>
@@ -147,9 +156,6 @@
   </si>
   <si>
     <t>output_comm</t>
-  </si>
-  <si>
-    <t>TRA_FT_HFO</t>
   </si>
   <si>
     <t>HH2_DEL_TRA_LH2_C_1_NEW</t>
@@ -558,7 +564,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -607,22 +613,22 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D2">
-        <v>0.582</v>
+        <v>0.5819999999999999</v>
       </c>
       <c r="E2">
         <v>0.334</v>
       </c>
       <c r="F2">
-        <v>0.264</v>
+        <v>0.3689999999999999</v>
       </c>
       <c r="G2">
-        <v>0.1460600635005933</v>
+        <v>0.1460600635007268</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>0.07303003175029658</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -645,7 +651,7 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -654,13 +660,13 @@
         <v>0.105</v>
       </c>
       <c r="F3">
-        <v>0.105</v>
+        <v>0</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3">
-        <v>0.0730300317502966</v>
+        <v>0</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -683,16 +689,16 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D4">
-        <v>3.548458638278998</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>2.838766910623198</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>2.129075182967398</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <v>1.419383455311599</v>
@@ -718,37 +724,37 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D5">
-        <v>198982.8156135253</v>
+        <v>3.548458638278998</v>
       </c>
       <c r="E5">
-        <v>204242.1749637213</v>
+        <v>2.838766910623198</v>
       </c>
       <c r="F5">
-        <v>176809.0812363035</v>
+        <v>2.129075182967398</v>
       </c>
       <c r="G5">
-        <v>229372.870751458</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>191828.4347297169</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>118852.1017272293</v>
+        <v>0</v>
       </c>
       <c r="J5">
-        <v>20160.00890140725</v>
+        <v>0</v>
       </c>
       <c r="K5">
-        <v>12337.94626304703</v>
+        <v>0</v>
       </c>
       <c r="L5">
-        <v>1565.086332553496</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -759,34 +765,34 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D6">
-        <v>7418.568219084142</v>
+        <v>198646.9297769822</v>
       </c>
       <c r="E6">
-        <v>14709.30790823598</v>
+        <v>204077.2881444494</v>
       </c>
       <c r="F6">
-        <v>19335.4262232156</v>
+        <v>176807.087842507</v>
       </c>
       <c r="G6">
-        <v>21526.79399099144</v>
+        <v>217373.8629505122</v>
       </c>
       <c r="H6">
-        <v>26165.95440800993</v>
+        <v>205586.2548122766</v>
       </c>
       <c r="I6">
-        <v>28754.99863628495</v>
+        <v>116208.3114562636</v>
       </c>
       <c r="J6">
-        <v>2926.452905042988</v>
+        <v>20979.00812860801</v>
       </c>
       <c r="K6">
-        <v>2884.195230322684</v>
+        <v>13015.63849066063</v>
       </c>
       <c r="L6">
-        <v>939.0517995320976</v>
+        <v>3042.754612000579</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -797,34 +803,34 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>7362.774462251439</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>14709.30790823524</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>18829.39407036373</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>21526.79399099141</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>26165.95440800994</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>28753.55601001736</v>
       </c>
       <c r="J7">
-        <v>60102.8394409051</v>
+        <v>3045.339889636644</v>
       </c>
       <c r="K7">
-        <v>67948.70543292888</v>
+        <v>3042.616790024563</v>
       </c>
       <c r="L7">
-        <v>20003.50253104742</v>
+        <v>1825.652767200345</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -835,7 +841,7 @@
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -844,25 +850,25 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>17006.0365338585</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>18361.78100303936</v>
+        <v>0</v>
       </c>
       <c r="H8">
-        <v>19466.33258359015</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <v>19466.33258359015</v>
+        <v>0</v>
       </c>
       <c r="J8">
-        <v>14359.12892074427</v>
+        <v>60208.00155443574</v>
       </c>
       <c r="K8">
-        <v>12968.99408445752</v>
+        <v>69473.45914121259</v>
       </c>
       <c r="L8">
-        <v>8794.085987936915</v>
+        <v>54769.58301601034</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -870,37 +876,37 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D9">
-        <v>241.4490648374262</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>242.1199363221268</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>232.161583327048</v>
+        <v>16971.64616675262</v>
       </c>
       <c r="G9">
-        <v>262.7649967022483</v>
+        <v>18361.78100303936</v>
       </c>
       <c r="H9">
-        <v>611.5562900097099</v>
+        <v>19466.33258359015</v>
       </c>
       <c r="I9">
-        <v>1007.650494806335</v>
+        <v>19466.33258359015</v>
       </c>
       <c r="J9">
-        <v>1088.739943476629</v>
+        <v>17278.98008187444</v>
       </c>
       <c r="K9">
-        <v>1377.531199642253</v>
+        <v>15888.8452455877</v>
       </c>
       <c r="L9">
-        <v>1696.504881919234</v>
+        <v>1217.101844800228</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -911,34 +917,34 @@
         <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D10">
-        <v>2.058542131979698</v>
+        <v>238.615166123246</v>
       </c>
       <c r="E10">
-        <v>8.076904107402811</v>
+        <v>239.3709460178159</v>
       </c>
       <c r="F10">
-        <v>11.33003728682171</v>
+        <v>205.8947286821706</v>
       </c>
       <c r="G10">
-        <v>39.0685286250268</v>
+        <v>235.8575914421443</v>
       </c>
       <c r="H10">
-        <v>168.6577354556589</v>
+        <v>643.5674989602056</v>
       </c>
       <c r="I10">
-        <v>425.6095355729003</v>
+        <v>1074.28051811402</v>
       </c>
       <c r="J10">
-        <v>625.8261300505758</v>
+        <v>817.4381753802699</v>
       </c>
       <c r="K10">
-        <v>1090.700880055701</v>
+        <v>898.8440527013404</v>
       </c>
       <c r="L10">
-        <v>1696.504881919234</v>
+        <v>849.6827419038478</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -946,37 +952,37 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D11">
-        <v>75161.48772542756</v>
+        <v>4.817864564207803</v>
       </c>
       <c r="E11">
-        <v>63058.06832603392</v>
+        <v>10.75355256160026</v>
       </c>
       <c r="F11">
-        <v>55542.63651569869</v>
+        <v>36.90565891472869</v>
       </c>
       <c r="G11">
-        <v>43918.95812426758</v>
+        <v>51.1217306268687</v>
       </c>
       <c r="H11">
-        <v>27559.44845161116</v>
+        <v>138.7314954442554</v>
       </c>
       <c r="I11">
-        <v>4877.669203698396</v>
+        <v>335.0123203351087</v>
       </c>
       <c r="J11">
-        <v>2981.470868606867</v>
+        <v>497.7416879125499</v>
       </c>
       <c r="K11">
-        <v>76.21218936394932</v>
+        <v>711.9875829641441</v>
       </c>
       <c r="L11">
-        <v>94.03398386871736</v>
+        <v>849.6827419038482</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -987,34 +993,34 @@
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D12">
-        <v>14059.61842364205</v>
+        <v>75161.48772542756</v>
       </c>
       <c r="E12">
-        <v>12056.38539063793</v>
+        <v>63113.41983672559</v>
       </c>
       <c r="F12">
-        <v>10619.47264199522</v>
+        <v>55544.7261084433</v>
       </c>
       <c r="G12">
-        <v>8397.083817470029</v>
+        <v>45711.39217491968</v>
       </c>
       <c r="H12">
-        <v>5269.227880056473</v>
+        <v>26973.55136390841</v>
       </c>
       <c r="I12">
-        <v>932.5858100152909</v>
+        <v>4291.98889574741</v>
       </c>
       <c r="J12">
-        <v>570.0422289663444</v>
+        <v>82.31730203967484</v>
       </c>
       <c r="K12">
-        <v>14.57138714883057</v>
+        <v>153.1306339397975</v>
       </c>
       <c r="L12">
-        <v>17.9788245887359</v>
+        <v>222.4881969949566</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1025,34 +1031,34 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D13">
-        <v>3276.383480154389</v>
+        <v>14059.61842364205</v>
       </c>
       <c r="E13">
-        <v>4203.871221735594</v>
+        <v>12051.64008346075</v>
       </c>
       <c r="F13">
-        <v>3702.842434379913</v>
+        <v>10619.87216161432</v>
       </c>
       <c r="G13">
-        <v>2927.930541617839</v>
+        <v>8244.006412685483</v>
       </c>
       <c r="H13">
-        <v>1837.296563440744</v>
+        <v>5157.207304797585</v>
       </c>
       <c r="I13">
-        <v>325.1779469132264</v>
+        <v>820.6066819542217</v>
       </c>
       <c r="J13">
-        <v>198.7647245737911</v>
+        <v>15.73865397488123</v>
       </c>
       <c r="K13">
-        <v>5.080812624263288</v>
+        <v>29.27780674069085</v>
       </c>
       <c r="L13">
-        <v>6.268932257914494</v>
+        <v>42.53862382796653</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1060,37 +1066,37 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D14">
-        <v>179.5189976813809</v>
+        <v>3276.383480154389</v>
       </c>
       <c r="E14">
-        <v>100.0509906883739</v>
+        <v>4122.045892055447</v>
       </c>
       <c r="F14">
-        <v>37.3515383330611</v>
+        <v>3702.981740562887</v>
       </c>
       <c r="G14">
-        <v>44.68282135770457</v>
+        <v>281.4857063782902</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>1798.236757593894</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>286.1325930498273</v>
       </c>
       <c r="J14">
-        <v>0</v>
+        <v>5.487820135978324</v>
       </c>
       <c r="K14">
-        <v>0</v>
+        <v>10.20870892931983</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>14.83254646633044</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1098,34 +1104,34 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D15">
-        <v>9.862565402026727</v>
+        <v>1593.262433190275</v>
       </c>
       <c r="E15">
-        <v>8.629744726773383</v>
+        <v>1960.168095430236</v>
       </c>
       <c r="F15">
-        <v>125.7548989382516</v>
+        <v>2035.489687669987</v>
       </c>
       <c r="G15">
-        <v>544.6918750569678</v>
+        <v>1456.497776385815</v>
       </c>
       <c r="H15">
-        <v>1064.423192185728</v>
+        <v>191.6843829439324</v>
       </c>
       <c r="I15">
-        <v>3303.532621003183</v>
+        <v>19.15619967634759</v>
       </c>
       <c r="J15">
-        <v>3118.691579497728</v>
+        <v>112.7175702814222</v>
       </c>
       <c r="K15">
-        <v>146.2491829300208</v>
+        <v>233.0635454739155</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -1139,31 +1145,31 @@
         <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D16">
-        <v>0.519082389580354</v>
+        <v>210.9982158669669</v>
       </c>
       <c r="E16">
-        <v>1.23282067525334</v>
+        <v>131.53020887396</v>
       </c>
       <c r="F16">
-        <v>31.83668327550674</v>
+        <v>37.35153833306109</v>
       </c>
       <c r="G16">
-        <v>280.0472365331455</v>
+        <v>76.1620395432906</v>
       </c>
       <c r="H16">
-        <v>980.3897822763289</v>
+        <v>0</v>
       </c>
       <c r="I16">
-        <v>1225.303906516373</v>
+        <v>0</v>
       </c>
       <c r="J16">
-        <v>1915.011843415477</v>
+        <v>0</v>
       </c>
       <c r="K16">
-        <v>1552.032145379815</v>
+        <v>0</v>
       </c>
       <c r="L16">
         <v>0</v>
@@ -1174,34 +1180,34 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>9.862565402026723</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>8.629744726773383</v>
       </c>
       <c r="F17">
-        <v>1.591834163775336</v>
+        <v>125.7548989382516</v>
       </c>
       <c r="G17">
-        <v>15.402598009323</v>
+        <v>103.2038159977958</v>
       </c>
       <c r="H17">
-        <v>56.02227327293309</v>
+        <v>710.2746622800996</v>
       </c>
       <c r="I17">
-        <v>164.2583196509684</v>
+        <v>3535.132100511202</v>
       </c>
       <c r="J17">
-        <v>228.0074721180197</v>
+        <v>2888.704140257516</v>
       </c>
       <c r="K17">
-        <v>92.52499328225839</v>
+        <v>70.22829067993366</v>
       </c>
       <c r="L17">
         <v>0</v>
@@ -1215,31 +1221,31 @@
         <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>0.5190823895803539</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>1.232820675253341</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>31.83668327550673</v>
       </c>
       <c r="G18">
-        <v>0.9899090011670063</v>
+        <v>53.06108791660456</v>
       </c>
       <c r="H18">
-        <v>6.152637391702759</v>
+        <v>654.2003468369338</v>
       </c>
       <c r="I18">
-        <v>38.31239935269515</v>
+        <v>1225.303906516375</v>
       </c>
       <c r="J18">
-        <v>225.4351405628443</v>
+        <v>1899.880167776573</v>
       </c>
       <c r="K18">
-        <v>0</v>
+        <v>745.2798194605206</v>
       </c>
       <c r="L18">
         <v>0</v>
@@ -1250,34 +1256,34 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D19">
-        <v>4.277305825242719</v>
+        <v>0</v>
       </c>
       <c r="E19">
-        <v>2.138652912621359</v>
+        <v>0</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>1.591834163775337</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>2.91835983541325</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>37.38287696211051</v>
       </c>
       <c r="I19">
-        <v>0</v>
+        <v>172.6583007730209</v>
       </c>
       <c r="J19">
-        <v>0</v>
+        <v>216.9045156949238</v>
       </c>
       <c r="K19">
-        <v>0</v>
+        <v>44.43014308322334</v>
       </c>
       <c r="L19">
         <v>0</v>
@@ -1288,10 +1294,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -1306,19 +1312,19 @@
         <v>0</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>6.152637391702759</v>
       </c>
       <c r="I20">
-        <v>0</v>
+        <v>38.31239935269516</v>
       </c>
       <c r="J20">
-        <v>23.00908787904872</v>
+        <v>225.4351405628443</v>
       </c>
       <c r="K20">
-        <v>0.3947082055076144</v>
+        <v>0</v>
       </c>
       <c r="L20">
-        <v>23.00908787904872</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1329,13 +1335,13 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>4.277305825242719</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>2.138652912621359</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -1350,13 +1356,13 @@
         <v>0</v>
       </c>
       <c r="J21">
-        <v>186.1644382941215</v>
+        <v>0</v>
       </c>
       <c r="K21">
-        <v>3.193548208197972</v>
+        <v>0</v>
       </c>
       <c r="L21">
-        <v>186.1644382941215</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -1367,7 +1373,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -1376,25 +1382,25 @@
         <v>0</v>
       </c>
       <c r="F22">
-        <v>0.172882497426718</v>
+        <v>0</v>
       </c>
       <c r="G22">
         <v>0</v>
       </c>
       <c r="H22">
-        <v>0.0211259765142098</v>
+        <v>0</v>
       </c>
       <c r="I22">
-        <v>4.702092510052073</v>
+        <v>4.680966533537863</v>
       </c>
       <c r="J22">
-        <v>4.702092510052073</v>
+        <v>27.69005441258658</v>
       </c>
       <c r="K22">
-        <v>4.683075435335134</v>
+        <v>27.69005441258658</v>
       </c>
       <c r="L22">
-        <v>105.6532955662002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -1405,7 +1411,7 @@
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -1420,19 +1426,19 @@
         <v>0</v>
       </c>
       <c r="H23">
-        <v>0.170928355433152</v>
+        <v>0</v>
       </c>
       <c r="I23">
-        <v>38.04420303587586</v>
+        <v>37.87327468044271</v>
       </c>
       <c r="J23">
-        <v>38.04420303587586</v>
+        <v>224.0377129745642</v>
       </c>
       <c r="K23">
-        <v>37.89033761316609</v>
+        <v>224.0377129745642</v>
       </c>
       <c r="L23">
-        <v>854.8312095810742</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -1443,7 +1449,7 @@
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -1452,25 +1458,101 @@
         <v>0</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>0.172882497426718</v>
       </c>
       <c r="G24">
         <v>0</v>
       </c>
       <c r="H24">
-        <v>0</v>
+        <v>0.0211259765142098</v>
       </c>
       <c r="I24">
+        <v>0.0211259765142098</v>
+      </c>
+      <c r="J24">
+        <v>0.0211259765142098</v>
+      </c>
+      <c r="K24">
+        <v>32.99942120684771</v>
+      </c>
+      <c r="L24">
+        <v>29.87833821718953</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0.170928355433152</v>
+      </c>
+      <c r="I25">
+        <v>0.170928355433152</v>
+      </c>
+      <c r="J25">
+        <v>0.170928355433152</v>
+      </c>
+      <c r="K25">
+        <v>266.9953170372224</v>
+      </c>
+      <c r="L25">
+        <v>241.7429183027154</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
         <v>0.9899090011670064</v>
       </c>
-      <c r="J24">
+      <c r="J26">
         <v>6.152637391702759</v>
       </c>
-      <c r="K24">
-        <v>38.31239935269517</v>
-      </c>
-      <c r="L24">
-        <v>225.4351405628443</v>
+      <c r="K26">
+        <v>38.31239935269515</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1491,7 +1573,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -1529,10 +1611,10 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D2">
-        <v>0.582</v>
+        <v>0.5819999999999999</v>
       </c>
       <c r="E2">
         <v>0.439</v>
@@ -1541,10 +1623,10 @@
         <v>0.3689999999999999</v>
       </c>
       <c r="G2">
-        <v>0.1460600635005933</v>
+        <v>0.1460600635007268</v>
       </c>
       <c r="H2">
-        <v>0.0730300317502966</v>
+        <v>0.07303003175029658</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1567,7 +1649,7 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D3">
         <v>3.548458638278998</v>
@@ -1605,34 +1687,34 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D4">
-        <v>8830.748095487703</v>
+        <v>8814.240635513537</v>
       </c>
       <c r="E4">
-        <v>9326.65791604474</v>
+        <v>9319.56778281603</v>
       </c>
       <c r="F4">
-        <v>9066.4668709098</v>
+        <v>9046.144789168373</v>
       </c>
       <c r="G4">
-        <v>11467.44318411311</v>
+        <v>10951.48584867244</v>
       </c>
       <c r="H4">
-        <v>10073.28164015216</v>
+        <v>10664.86790370223</v>
       </c>
       <c r="I4">
-        <v>7031.09395749137</v>
+        <v>6917.357598667941</v>
       </c>
       <c r="J4">
-        <v>4251.485748159676</v>
+        <v>4424.202117444348</v>
       </c>
       <c r="K4">
-        <v>4197.625691597962</v>
+        <v>4428.190669348526</v>
       </c>
       <c r="L4">
-        <v>1369.137523717798</v>
+        <v>2661.801734578102</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1643,7 +1725,7 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D5">
         <v>225.296</v>
@@ -1655,22 +1737,22 @@
         <v>225.513</v>
       </c>
       <c r="G5">
-        <v>280.1727241433552</v>
+        <v>266.7339161795088</v>
       </c>
       <c r="H5">
-        <v>725.9144169418577</v>
+        <v>727.0948572102327</v>
       </c>
       <c r="I5">
-        <v>1336.405766490116</v>
+        <v>1311.971183573822</v>
       </c>
       <c r="J5">
-        <v>1601.619271263929</v>
+        <v>1228.984915743672</v>
       </c>
       <c r="K5">
-        <v>2310.382195722</v>
+        <v>1507.818952564677</v>
       </c>
       <c r="L5">
-        <v>3180.946653598565</v>
+        <v>1593.155141069715</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1681,34 +1763,34 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D6">
-        <v>3826.552589408666</v>
+        <v>3826.552589408667</v>
       </c>
       <c r="E6">
         <v>3259.031335069285</v>
       </c>
       <c r="F6">
-        <v>2870.611131015129</v>
+        <v>2870.719127476374</v>
       </c>
       <c r="G6">
-        <v>2269.864341396109</v>
+        <v>2269.974208450437</v>
       </c>
       <c r="H6">
-        <v>1424.355494314213</v>
+        <v>1394.07456407581</v>
       </c>
       <c r="I6">
-        <v>252.0926694862386</v>
+        <v>221.8229430798359</v>
       </c>
       <c r="J6">
-        <v>154.091415156376</v>
+        <v>4.254406674473155</v>
       </c>
       <c r="K6">
-        <v>3.938876020862829</v>
+        <v>7.914253443167797</v>
       </c>
       <c r="L6">
-        <v>4.859960162513031</v>
+        <v>11.49886168318085</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1716,22 +1798,22 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D7">
-        <v>1605.070043182009</v>
+        <v>1593.262433190275</v>
       </c>
       <c r="E7">
-        <v>1981.395153867322</v>
+        <v>1960.168095430236</v>
       </c>
       <c r="F7">
         <v>2035.489687669987</v>
       </c>
       <c r="G7">
-        <v>383.3687658878648</v>
+        <v>1456.497776385815</v>
       </c>
       <c r="H7">
         <v>191.6843829439324</v>
@@ -1743,10 +1825,10 @@
         <v>112.7175702814222</v>
       </c>
       <c r="K7">
-        <v>0</v>
+        <v>233.0635454739155</v>
       </c>
       <c r="L7">
-        <v>413.9949531830487</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1754,22 +1836,22 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D8">
-        <v>179.5189976813809</v>
+        <v>210.9982158669669</v>
       </c>
       <c r="E8">
-        <v>100.0509906883739</v>
+        <v>131.53020887396</v>
       </c>
       <c r="F8">
-        <v>37.3515383330611</v>
+        <v>37.35153833306109</v>
       </c>
       <c r="G8">
-        <v>44.68282135770457</v>
+        <v>76.1620395432906</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1792,10 +1874,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D9">
         <v>10.29859460927422</v>
@@ -1807,19 +1889,19 @@
         <v>158.081</v>
       </c>
       <c r="G9">
-        <v>834.7605630042511</v>
+        <v>158.081</v>
       </c>
       <c r="H9">
-        <v>2088.074685242437</v>
+        <v>1393.478901891148</v>
       </c>
       <c r="I9">
-        <v>4666.260300542878</v>
+        <v>4905.548550475132</v>
       </c>
       <c r="J9">
-        <v>5232.035090353493</v>
+        <v>4977.582358546221</v>
       </c>
       <c r="K9">
-        <v>1781.109308481964</v>
+        <v>855.1782243109195</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -1830,10 +1912,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1845,13 +1927,13 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>0.9899090011670063</v>
+        <v>0</v>
       </c>
       <c r="H10">
         <v>6.152637391702759</v>
       </c>
       <c r="I10">
-        <v>38.31239935269515</v>
+        <v>38.31239935269516</v>
       </c>
       <c r="J10">
         <v>225.4351405628443</v>
@@ -1868,10 +1950,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D11">
         <v>4.277305825242719</v>
@@ -1906,10 +1988,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1927,16 +2009,16 @@
         <v>0</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>19.61750519964504</v>
       </c>
       <c r="J12">
-        <v>96.42899556583146</v>
+        <v>116.0465007654765</v>
       </c>
       <c r="K12">
-        <v>1.654186206718276</v>
+        <v>116.0465007654765</v>
       </c>
       <c r="L12">
-        <v>96.42899556583146</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1944,10 +2026,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1962,19 +2044,19 @@
         <v>0</v>
       </c>
       <c r="H13">
-        <v>0.08853704702773381</v>
+        <v>0.08853704702773382</v>
       </c>
       <c r="I13">
-        <v>19.70604224667278</v>
+        <v>0.08853704702773382</v>
       </c>
       <c r="J13">
-        <v>19.70604224667278</v>
+        <v>0.08853704702773382</v>
       </c>
       <c r="K13">
-        <v>19.62634341535906</v>
+        <v>138.2975743305163</v>
       </c>
       <c r="L13">
-        <v>442.7833568728934</v>
+        <v>125.2173992556762</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1982,10 +2064,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -2009,10 +2091,10 @@
         <v>6.152637391702759</v>
       </c>
       <c r="K14">
-        <v>38.31239935269517</v>
+        <v>38.31239935269515</v>
       </c>
       <c r="L14">
-        <v>225.4351405628443</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -2020,10 +2102,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -2038,19 +2120,19 @@
         <v>0</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>0.008705114254624592</v>
       </c>
       <c r="I15">
-        <v>0.9379261261528213</v>
+        <v>0.008705114254625744</v>
       </c>
       <c r="J15">
-        <v>5.88872210961464</v>
+        <v>4.959501097716443</v>
       </c>
       <c r="K15">
-        <v>36.71525896327071</v>
+        <v>4.959501097716444</v>
       </c>
       <c r="L15">
-        <v>216.1033327415355</v>
+        <v>184.8078328248031</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -2058,10 +2140,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -2076,19 +2158,19 @@
         <v>0</v>
       </c>
       <c r="H16">
-        <v>0.00870511425462459</v>
+        <v>0</v>
       </c>
       <c r="I16">
-        <v>0.008705114254624557</v>
+        <v>0.9379261261528165</v>
       </c>
       <c r="J16">
-        <v>0.008705114254624471</v>
+        <v>0.9379261261528156</v>
       </c>
       <c r="K16">
-        <v>0.008705114254624592</v>
+        <v>31.76446297980888</v>
       </c>
       <c r="L16">
-        <v>0</v>
+        <v>31.29549991673247</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -2096,10 +2178,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -2111,22 +2193,22 @@
         <v>0</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>2.656993306345552</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>2.656993306345552</v>
       </c>
       <c r="I17">
-        <v>22.54219698339416</v>
+        <v>61.90398783067038</v>
       </c>
       <c r="J17">
-        <v>633.6580776784569</v>
+        <v>1312.921944357951</v>
       </c>
       <c r="K17">
-        <v>1191.55474771288</v>
+        <v>2422.596622819986</v>
       </c>
       <c r="L17">
-        <v>1339.118844065566</v>
+        <v>3394.965348299032</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Addition of the elastic run and update of results analysis
</commit_message>
<xml_diff>
--- a/TEMOA_Europe_Results/_1_Transport_fueltechs.xlsx
+++ b/TEMOA_Europe_Results/_1_Transport_fueltechs.xlsx
@@ -616,19 +616,19 @@
         <v>24</v>
       </c>
       <c r="D2">
-        <v>0.5819999999999999</v>
+        <v>0.291</v>
       </c>
       <c r="E2">
-        <v>0.334</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>0.3689999999999999</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>0.1460600635007268</v>
+        <v>0.1387570603255635</v>
       </c>
       <c r="H2">
-        <v>0.07303003175029658</v>
+        <v>0</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -654,19 +654,19 @@
         <v>25</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>0.291</v>
       </c>
       <c r="E3">
-        <v>0.105</v>
+        <v>0.439</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>0.369</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>0.06937853016278178</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -695,16 +695,16 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>2.838766910623198</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>2.129075182967398</v>
       </c>
       <c r="G4">
         <v>1.419383455311599</v>
       </c>
       <c r="H4">
-        <v>0.7096917276557995</v>
+        <v>0</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -733,16 +733,16 @@
         <v>3.548458638278998</v>
       </c>
       <c r="E5">
-        <v>2.838766910623198</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>2.129075182967398</v>
+        <v>0</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>0.7096917276557995</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -768,31 +768,31 @@
         <v>28</v>
       </c>
       <c r="D6">
-        <v>198646.9297769822</v>
+        <v>192916.6738549898</v>
       </c>
       <c r="E6">
-        <v>204077.2881444494</v>
+        <v>210970.1272594048</v>
       </c>
       <c r="F6">
-        <v>176807.087842507</v>
+        <v>166736.5233268229</v>
       </c>
       <c r="G6">
-        <v>217373.8629505122</v>
+        <v>242931.3367324624</v>
       </c>
       <c r="H6">
-        <v>205586.2548122766</v>
+        <v>214673.3958739777</v>
       </c>
       <c r="I6">
-        <v>116208.3114562636</v>
+        <v>112413.8842600082</v>
       </c>
       <c r="J6">
-        <v>20979.00812860801</v>
+        <v>20650.28433098331</v>
       </c>
       <c r="K6">
-        <v>13015.63849066063</v>
+        <v>13487.53212053503</v>
       </c>
       <c r="L6">
-        <v>3042.754612000579</v>
+        <v>2818.130988676962</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -806,31 +806,31 @@
         <v>29</v>
       </c>
       <c r="D7">
-        <v>7362.774462251439</v>
+        <v>14780.70269999836</v>
       </c>
       <c r="E7">
-        <v>14709.30790823524</v>
+        <v>16944.47835473503</v>
       </c>
       <c r="F7">
-        <v>18829.39407036373</v>
+        <v>22345.38578261545</v>
       </c>
       <c r="G7">
-        <v>21526.79399099141</v>
+        <v>17199.51802080974</v>
       </c>
       <c r="H7">
-        <v>26165.95440800994</v>
+        <v>26165.95440801004</v>
       </c>
       <c r="I7">
-        <v>28753.55601001736</v>
+        <v>4353.302492789441</v>
       </c>
       <c r="J7">
-        <v>3045.339889636644</v>
+        <v>2997.621919013707</v>
       </c>
       <c r="K7">
-        <v>3042.616790024563</v>
+        <v>3152.929586618577</v>
       </c>
       <c r="L7">
-        <v>1825.652767200345</v>
+        <v>1690.878593206179</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -847,10 +847,10 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>1064.831612009241</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>6725.252286374135</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -859,16 +859,16 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>8876.563756593521</v>
       </c>
       <c r="J8">
-        <v>60208.00155443574</v>
+        <v>57092.07505593903</v>
       </c>
       <c r="K8">
-        <v>69473.45914121259</v>
+        <v>70658.16024421096</v>
       </c>
       <c r="L8">
-        <v>54769.58301601034</v>
+        <v>50726.35779618536</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -888,7 +888,7 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>16971.64616675262</v>
+        <v>17006.0365338585</v>
       </c>
       <c r="G9">
         <v>18361.78100303936</v>
@@ -900,13 +900,13 @@
         <v>19466.33258359015</v>
       </c>
       <c r="J9">
-        <v>17278.98008187444</v>
+        <v>19180.74932785417</v>
       </c>
       <c r="K9">
-        <v>15888.8452455877</v>
+        <v>17799.03093592133</v>
       </c>
       <c r="L9">
-        <v>1217.101844800228</v>
+        <v>1127.252395470788</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -920,31 +920,31 @@
         <v>32</v>
       </c>
       <c r="D10">
-        <v>238.615166123246</v>
+        <v>247.2053541453888</v>
       </c>
       <c r="E10">
-        <v>239.3709460178159</v>
+        <v>252.4680876084153</v>
       </c>
       <c r="F10">
-        <v>205.8947286821706</v>
+        <v>236.8561238959894</v>
       </c>
       <c r="G10">
-        <v>235.8575914421443</v>
+        <v>216.2603955202925</v>
       </c>
       <c r="H10">
-        <v>643.5674989602056</v>
+        <v>603.826992792788</v>
       </c>
       <c r="I10">
-        <v>1074.28051811402</v>
+        <v>917.3119876812468</v>
       </c>
       <c r="J10">
-        <v>817.4381753802699</v>
+        <v>780.2207363646929</v>
       </c>
       <c r="K10">
-        <v>898.8440527013404</v>
+        <v>897.5870941873752</v>
       </c>
       <c r="L10">
-        <v>849.6827419038478</v>
+        <v>865.7888843438553</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -958,31 +958,31 @@
         <v>33</v>
       </c>
       <c r="D11">
-        <v>4.817864564207803</v>
+        <v>2.959138178052658</v>
       </c>
       <c r="E11">
-        <v>10.75355256160026</v>
+        <v>4.644969634132857</v>
       </c>
       <c r="F11">
-        <v>36.90565891472869</v>
+        <v>12.99209315116792</v>
       </c>
       <c r="G11">
-        <v>51.1217306268687</v>
+        <v>47.43384644502824</v>
       </c>
       <c r="H11">
-        <v>138.7314954442554</v>
+        <v>188.0816000012074</v>
       </c>
       <c r="I11">
-        <v>335.0123203351087</v>
+        <v>434.3660050120391</v>
       </c>
       <c r="J11">
-        <v>497.7416879125499</v>
+        <v>464.2004285862787</v>
       </c>
       <c r="K11">
-        <v>711.9875829641441</v>
+        <v>696.292634828991</v>
       </c>
       <c r="L11">
-        <v>849.6827419038482</v>
+        <v>865.7888843438554</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -996,31 +996,31 @@
         <v>34</v>
       </c>
       <c r="D12">
-        <v>75161.48772542756</v>
+        <v>74741.53624898972</v>
       </c>
       <c r="E12">
-        <v>63113.41983672559</v>
+        <v>61982.42202692643</v>
       </c>
       <c r="F12">
-        <v>55544.7261084433</v>
+        <v>55542.63651569869</v>
       </c>
       <c r="G12">
-        <v>45711.39217491968</v>
+        <v>42540.20368103011</v>
       </c>
       <c r="H12">
-        <v>26973.55136390841</v>
+        <v>13457.30601074946</v>
       </c>
       <c r="I12">
-        <v>4291.98889574741</v>
+        <v>12774.14483266342</v>
       </c>
       <c r="J12">
-        <v>82.31730203967484</v>
+        <v>460.9610785447496</v>
       </c>
       <c r="K12">
-        <v>153.1306339397975</v>
+        <v>151.9050674479426</v>
       </c>
       <c r="L12">
-        <v>222.4881969949566</v>
+        <v>218.347628920442</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1034,31 +1034,31 @@
         <v>35</v>
       </c>
       <c r="D13">
-        <v>14059.61842364205</v>
+        <v>14095.62103188714</v>
       </c>
       <c r="E13">
-        <v>12051.64008346075</v>
+        <v>11850.72723030543</v>
       </c>
       <c r="F13">
-        <v>10619.87216161432</v>
+        <v>10619.47264199522</v>
       </c>
       <c r="G13">
-        <v>8244.006412685483</v>
+        <v>8133.472905052301</v>
       </c>
       <c r="H13">
-        <v>5157.207304797585</v>
+        <v>2572.969199539521</v>
       </c>
       <c r="I13">
-        <v>820.6066819542217</v>
+        <v>2442.352219578415</v>
       </c>
       <c r="J13">
-        <v>15.73865397488123</v>
+        <v>88.13343891673202</v>
       </c>
       <c r="K13">
-        <v>29.27780674069085</v>
+        <v>29.04348459382046</v>
       </c>
       <c r="L13">
-        <v>42.53862382796653</v>
+        <v>41.74696804516627</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1072,31 +1072,31 @@
         <v>36</v>
       </c>
       <c r="D14">
-        <v>3276.383480154389</v>
+        <v>3897.191613117493</v>
       </c>
       <c r="E14">
-        <v>4122.045892055447</v>
+        <v>4132.161468461761</v>
       </c>
       <c r="F14">
-        <v>3702.981740562887</v>
+        <v>3702.842434379913</v>
       </c>
       <c r="G14">
-        <v>281.4857063782902</v>
+        <v>2836.013578735341</v>
       </c>
       <c r="H14">
-        <v>1798.236757593894</v>
+        <v>897.153734049964</v>
       </c>
       <c r="I14">
-        <v>286.1325930498273</v>
+        <v>851.6096555108948</v>
       </c>
       <c r="J14">
-        <v>5.487820135978324</v>
+        <v>30.73073856964998</v>
       </c>
       <c r="K14">
-        <v>10.20870892931983</v>
+        <v>10.1270044965295</v>
       </c>
       <c r="L14">
-        <v>14.83254646633044</v>
+        <v>14.55650859469613</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1110,28 +1110,28 @@
         <v>37</v>
       </c>
       <c r="D15">
-        <v>1593.262433190275</v>
+        <v>910.5008189836789</v>
       </c>
       <c r="E15">
-        <v>1960.168095430236</v>
+        <v>757.64294283116</v>
       </c>
       <c r="F15">
-        <v>2035.489687669987</v>
+        <v>1663.738980971423</v>
       </c>
       <c r="G15">
-        <v>1456.497776385815</v>
+        <v>364.6705343690258</v>
       </c>
       <c r="H15">
-        <v>191.6843829439324</v>
+        <v>182.1001637967357</v>
       </c>
       <c r="I15">
-        <v>19.15619967634759</v>
+        <v>18.19838969253021</v>
       </c>
       <c r="J15">
-        <v>112.7175702814222</v>
+        <v>107.0816917673511</v>
       </c>
       <c r="K15">
-        <v>233.0635454739155</v>
+        <v>108.4417981664033</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -1148,16 +1148,16 @@
         <v>38</v>
       </c>
       <c r="D16">
-        <v>210.9982158669669</v>
+        <v>215.7244202622394</v>
       </c>
       <c r="E16">
-        <v>131.53020887396</v>
+        <v>67.70714091025418</v>
       </c>
       <c r="F16">
-        <v>37.35153833306109</v>
+        <v>8.698905109489051</v>
       </c>
       <c r="G16">
-        <v>76.1620395432906</v>
+        <v>15.03369881730334</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -1186,28 +1186,28 @@
         <v>39</v>
       </c>
       <c r="D17">
-        <v>9.862565402026723</v>
+        <v>51.2022008834085</v>
       </c>
       <c r="E17">
-        <v>8.629744726773383</v>
+        <v>136.0671654928556</v>
       </c>
       <c r="F17">
-        <v>125.7548989382516</v>
+        <v>127.2946502852885</v>
       </c>
       <c r="G17">
-        <v>103.2038159977958</v>
+        <v>103.0385147360157</v>
       </c>
       <c r="H17">
-        <v>710.2746622800996</v>
+        <v>434.9257766255786</v>
       </c>
       <c r="I17">
-        <v>3535.132100511202</v>
+        <v>3481.229639198534</v>
       </c>
       <c r="J17">
-        <v>2888.704140257516</v>
+        <v>2424.068808726991</v>
       </c>
       <c r="K17">
-        <v>70.22829067993366</v>
+        <v>53.74897660246722</v>
       </c>
       <c r="L17">
         <v>0</v>
@@ -1224,28 +1224,28 @@
         <v>40</v>
       </c>
       <c r="D18">
-        <v>0.5190823895803539</v>
+        <v>2.694852678074132</v>
       </c>
       <c r="E18">
-        <v>1.232820675253341</v>
+        <v>19.43816649897937</v>
       </c>
       <c r="F18">
-        <v>31.83668327550673</v>
+        <v>31.82366257132213</v>
       </c>
       <c r="G18">
-        <v>53.06108791660456</v>
+        <v>52.97610012134483</v>
       </c>
       <c r="H18">
-        <v>654.2003468369338</v>
+        <v>400.5895311025066</v>
       </c>
       <c r="I18">
-        <v>1225.303906516375</v>
+        <v>1202.450784056603</v>
       </c>
       <c r="J18">
-        <v>1899.880167776573</v>
+        <v>2041.31149278085</v>
       </c>
       <c r="K18">
-        <v>745.2798194605206</v>
+        <v>570.3973027200665</v>
       </c>
       <c r="L18">
         <v>0</v>
@@ -1268,22 +1268,22 @@
         <v>0</v>
       </c>
       <c r="F19">
-        <v>1.591834163775337</v>
+        <v>0</v>
       </c>
       <c r="G19">
-        <v>2.91835983541325</v>
+        <v>2.913685506673966</v>
       </c>
       <c r="H19">
-        <v>37.38287696211051</v>
+        <v>22.89083034871465</v>
       </c>
       <c r="I19">
-        <v>172.6583007730209</v>
+        <v>169.8744194963003</v>
       </c>
       <c r="J19">
-        <v>216.9045156949238</v>
+        <v>202.2646129602856</v>
       </c>
       <c r="K19">
-        <v>44.43014308322334</v>
+        <v>34.00445458523485</v>
       </c>
       <c r="L19">
         <v>0</v>
@@ -1306,19 +1306,19 @@
         <v>0</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>0.1514277794960627</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>0.9404135511086561</v>
       </c>
       <c r="H20">
-        <v>6.152637391702759</v>
+        <v>5.845005522117619</v>
       </c>
       <c r="I20">
-        <v>38.31239935269516</v>
+        <v>36.39677938506041</v>
       </c>
       <c r="J20">
-        <v>225.4351405628443</v>
+        <v>214.1633835347021</v>
       </c>
       <c r="K20">
         <v>0</v>
@@ -1382,7 +1382,7 @@
         <v>0</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>0.1642383725553879</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -1391,16 +1391,16 @@
         <v>0</v>
       </c>
       <c r="I22">
-        <v>4.680966533537863</v>
+        <v>4.372857261038206</v>
       </c>
       <c r="J22">
-        <v>27.69005441258658</v>
+        <v>26.23149074613449</v>
       </c>
       <c r="K22">
-        <v>27.69005441258658</v>
+        <v>26.2134245251534</v>
       </c>
       <c r="L22">
-        <v>0</v>
+        <v>23.99259870269209</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -1423,22 +1423,22 @@
         <v>0</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>0.1642383725553879</v>
       </c>
       <c r="H23">
         <v>0</v>
       </c>
       <c r="I23">
-        <v>37.87327468044271</v>
+        <v>35.38039056658186</v>
       </c>
       <c r="J23">
-        <v>224.0377129745642</v>
+        <v>212.2366069459972</v>
       </c>
       <c r="K23">
-        <v>224.0377129745642</v>
+        <v>212.0904347944229</v>
       </c>
       <c r="L23">
-        <v>0</v>
+        <v>194.1219349581451</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -1458,25 +1458,25 @@
         <v>0</v>
       </c>
       <c r="F24">
-        <v>0.172882497426718</v>
+        <v>0</v>
       </c>
       <c r="G24">
         <v>0</v>
       </c>
       <c r="H24">
-        <v>0.0211259765142098</v>
+        <v>0.02006967768849931</v>
       </c>
       <c r="I24">
-        <v>0.0211259765142098</v>
+        <v>0.09413062351126328</v>
       </c>
       <c r="J24">
-        <v>0.0211259765142098</v>
+        <v>0.09413062351126328</v>
       </c>
       <c r="K24">
-        <v>32.99942120684771</v>
+        <v>4.485953227149231</v>
       </c>
       <c r="L24">
-        <v>29.87833821718953</v>
+        <v>4.391822603637968</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -1499,22 +1499,22 @@
         <v>0</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>0.8557329410114844</v>
       </c>
       <c r="H25">
-        <v>0.170928355433152</v>
+        <v>0.1623819376614945</v>
       </c>
       <c r="I25">
-        <v>0.170928355433152</v>
+        <v>0.7616023175002212</v>
       </c>
       <c r="J25">
-        <v>0.170928355433152</v>
+        <v>0.7616023175002212</v>
       </c>
       <c r="K25">
-        <v>266.9953170372224</v>
+        <v>36.29543974693469</v>
       </c>
       <c r="L25">
-        <v>241.7429183027154</v>
+        <v>35.53383742943447</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -1540,16 +1540,16 @@
         <v>0</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>0.1514277794960627</v>
       </c>
       <c r="I26">
-        <v>0.9899090011670064</v>
+        <v>0.9404135511086561</v>
       </c>
       <c r="J26">
-        <v>6.152637391702759</v>
+        <v>5.845005522117619</v>
       </c>
       <c r="K26">
-        <v>38.31239935269515</v>
+        <v>36.39677938506041</v>
       </c>
       <c r="L26">
         <v>0</v>
@@ -1614,19 +1614,19 @@
         <v>50</v>
       </c>
       <c r="D2">
-        <v>0.5819999999999999</v>
+        <v>0.582</v>
       </c>
       <c r="E2">
         <v>0.439</v>
       </c>
       <c r="F2">
-        <v>0.3689999999999999</v>
+        <v>0.369</v>
       </c>
       <c r="G2">
-        <v>0.1460600635007268</v>
+        <v>0.1387570603255635</v>
       </c>
       <c r="H2">
-        <v>0.07303003175029658</v>
+        <v>0.06937853016278178</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1690,31 +1690,31 @@
         <v>52</v>
       </c>
       <c r="D4">
-        <v>8814.240635513537</v>
+        <v>8842.302975664505</v>
       </c>
       <c r="E4">
-        <v>9319.56778281603</v>
+        <v>9745.513762208007</v>
       </c>
       <c r="F4">
-        <v>9046.144789168373</v>
+        <v>9040.626485100391</v>
       </c>
       <c r="G4">
-        <v>10951.48584867244</v>
+        <v>11890.34801039957</v>
       </c>
       <c r="H4">
-        <v>10664.86790370223</v>
+        <v>11055.61496935538</v>
       </c>
       <c r="I4">
-        <v>6917.357598667941</v>
+        <v>6241.956654381645</v>
       </c>
       <c r="J4">
-        <v>4424.202117444348</v>
+        <v>4354.878510122691</v>
       </c>
       <c r="K4">
-        <v>4428.190669348526</v>
+        <v>4588.738687813712</v>
       </c>
       <c r="L4">
-        <v>2661.801734578102</v>
+        <v>2465.300988894608</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1728,7 +1728,7 @@
         <v>53</v>
       </c>
       <c r="D5">
-        <v>225.296</v>
+        <v>225.2959999999999</v>
       </c>
       <c r="E5">
         <v>231.634</v>
@@ -1737,22 +1737,22 @@
         <v>225.513</v>
       </c>
       <c r="G5">
-        <v>266.7339161795088</v>
+        <v>239.6965100910401</v>
       </c>
       <c r="H5">
-        <v>727.0948572102327</v>
+        <v>722.1218135146563</v>
       </c>
       <c r="I5">
-        <v>1311.971183573822</v>
+        <v>1238.228493674559</v>
       </c>
       <c r="J5">
-        <v>1228.984915743672</v>
+        <v>1143.189069885189</v>
       </c>
       <c r="K5">
-        <v>1507.818952564677</v>
+        <v>1469.306387856179</v>
       </c>
       <c r="L5">
-        <v>1593.155141069715</v>
+        <v>1601.709436036133</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1769,28 +1769,28 @@
         <v>3826.552589408667</v>
       </c>
       <c r="E6">
-        <v>3259.031335069285</v>
+        <v>3203.4386870973</v>
       </c>
       <c r="F6">
-        <v>2870.719127476374</v>
+        <v>2870.611131015129</v>
       </c>
       <c r="G6">
-        <v>2269.974208450437</v>
+        <v>2198.606149492032</v>
       </c>
       <c r="H6">
-        <v>1394.07456407581</v>
+        <v>695.5142004649985</v>
       </c>
       <c r="I6">
-        <v>221.8229430798359</v>
+        <v>660.2063684081443</v>
       </c>
       <c r="J6">
-        <v>4.254406674473155</v>
+        <v>23.82386011980714</v>
       </c>
       <c r="K6">
-        <v>7.914253443167797</v>
+        <v>7.850912467045363</v>
       </c>
       <c r="L6">
-        <v>11.49886168318085</v>
+        <v>11.28486462526178</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1804,28 +1804,28 @@
         <v>55</v>
       </c>
       <c r="D7">
-        <v>1593.262433190275</v>
+        <v>910.5008189836789</v>
       </c>
       <c r="E7">
-        <v>1960.168095430236</v>
+        <v>757.64294283116</v>
       </c>
       <c r="F7">
-        <v>2035.489687669987</v>
+        <v>1663.738980971423</v>
       </c>
       <c r="G7">
-        <v>1456.497776385815</v>
+        <v>364.6705343690258</v>
       </c>
       <c r="H7">
-        <v>191.6843829439324</v>
+        <v>182.1001637967357</v>
       </c>
       <c r="I7">
-        <v>19.15619967634759</v>
+        <v>18.19838969253021</v>
       </c>
       <c r="J7">
-        <v>112.7175702814222</v>
+        <v>107.0816917673511</v>
       </c>
       <c r="K7">
-        <v>233.0635454739155</v>
+        <v>108.4417981664033</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -1842,16 +1842,16 @@
         <v>56</v>
       </c>
       <c r="D8">
-        <v>210.9982158669669</v>
+        <v>215.7244202622394</v>
       </c>
       <c r="E8">
-        <v>131.53020887396</v>
+        <v>67.70714091025418</v>
       </c>
       <c r="F8">
-        <v>37.35153833306109</v>
+        <v>8.698905109489051</v>
       </c>
       <c r="G8">
-        <v>76.1620395432906</v>
+        <v>15.03369881730334</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1880,28 +1880,28 @@
         <v>57</v>
       </c>
       <c r="D9">
-        <v>10.29859460927422</v>
+        <v>53.48897587023141</v>
       </c>
       <c r="E9">
-        <v>9.783664878810509</v>
+        <v>154.325</v>
       </c>
       <c r="F9">
-        <v>158.081</v>
+        <v>157.929572220504</v>
       </c>
       <c r="G9">
-        <v>158.081</v>
+        <v>157.929572220504</v>
       </c>
       <c r="H9">
-        <v>1393.478901891148</v>
+        <v>853.3796387440843</v>
       </c>
       <c r="I9">
-        <v>4905.548550475132</v>
+        <v>4827.211827159916</v>
       </c>
       <c r="J9">
-        <v>4977.582358546221</v>
+        <v>4638.06210498095</v>
       </c>
       <c r="K9">
-        <v>855.1782243109195</v>
+        <v>654.7105034631414</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -1924,19 +1924,19 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>0.1514277794960627</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>0.9404135511086561</v>
       </c>
       <c r="H10">
-        <v>6.152637391702759</v>
+        <v>5.845005522117619</v>
       </c>
       <c r="I10">
-        <v>38.31239935269516</v>
+        <v>36.39677938506041</v>
       </c>
       <c r="J10">
-        <v>225.4351405628443</v>
+        <v>214.1633835347021</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -2000,25 +2000,25 @@
         <v>0</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>0.07571388974803384</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>0.07571388974803384</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12">
-        <v>19.61750519964504</v>
+        <v>18.32624724853285</v>
       </c>
       <c r="J12">
-        <v>116.0465007654765</v>
+        <v>109.9337930360727</v>
       </c>
       <c r="K12">
-        <v>116.0465007654765</v>
+        <v>109.8580791463247</v>
       </c>
       <c r="L12">
-        <v>0</v>
+        <v>100.5508000176459</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -2038,25 +2038,25 @@
         <v>0</v>
       </c>
       <c r="F13">
-        <v>0.07969883131371704</v>
+        <v>0</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>0.3944928858062944</v>
       </c>
       <c r="H13">
-        <v>0.08853704702773382</v>
+        <v>0.08411019467634716</v>
       </c>
       <c r="I13">
-        <v>0.08853704702773382</v>
+        <v>0.3944928858062943</v>
       </c>
       <c r="J13">
-        <v>0.08853704702773382</v>
+        <v>0.3944928858062943</v>
       </c>
       <c r="K13">
-        <v>138.2975743305163</v>
+        <v>18.80022216105269</v>
       </c>
       <c r="L13">
-        <v>125.2173992556762</v>
+        <v>18.4057292752464</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -2082,16 +2082,16 @@
         <v>0</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>0.1514277794960627</v>
       </c>
       <c r="I14">
-        <v>0.9899090011670064</v>
+        <v>0.9404135511086561</v>
       </c>
       <c r="J14">
-        <v>6.152637391702759</v>
+        <v>5.845005522117619</v>
       </c>
       <c r="K14">
-        <v>38.31239935269515</v>
+        <v>36.39677938506041</v>
       </c>
       <c r="L14">
         <v>0</v>
@@ -2120,19 +2120,19 @@
         <v>0</v>
       </c>
       <c r="H15">
-        <v>0.008705114254624592</v>
+        <v>0.1448054107355396</v>
       </c>
       <c r="I15">
-        <v>0.008705114254625744</v>
+        <v>0.8992996783870737</v>
       </c>
       <c r="J15">
-        <v>4.959501097716443</v>
+        <v>0.8992996783870743</v>
       </c>
       <c r="K15">
-        <v>4.959501097716444</v>
+        <v>0.8992996783870748</v>
       </c>
       <c r="L15">
-        <v>184.8078328248031</v>
+        <v>171.3325081900247</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -2161,16 +2161,16 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <v>0.9379261261528165</v>
+        <v>0</v>
       </c>
       <c r="J16">
-        <v>0.9379261261528156</v>
+        <v>4.703958254495745</v>
       </c>
       <c r="K16">
-        <v>31.76446297980888</v>
+        <v>33.99284063270574</v>
       </c>
       <c r="L16">
-        <v>31.29549991673247</v>
+        <v>33.99284063270575</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -2193,22 +2193,22 @@
         <v>0</v>
       </c>
       <c r="G17">
-        <v>2.656993306345552</v>
+        <v>0.3868989205103038</v>
       </c>
       <c r="H17">
-        <v>2.656993306345552</v>
+        <v>2.292722269632621</v>
       </c>
       <c r="I17">
-        <v>61.90398783067038</v>
+        <v>21.9462113051214</v>
       </c>
       <c r="J17">
-        <v>1312.921944357951</v>
+        <v>1401.067707571761</v>
       </c>
       <c r="K17">
-        <v>2422.596622819986</v>
+        <v>2404.387869716356</v>
       </c>
       <c r="L17">
-        <v>3394.965348299032</v>
+        <v>3336.969172259398</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update postprocessing of results
</commit_message>
<xml_diff>
--- a/TEMOA_Europe_Results/_1_Transport_fueltechs.xlsx
+++ b/TEMOA_Europe_Results/_1_Transport_fueltechs.xlsx
@@ -695,7 +695,7 @@
         <v>204516.9717943329</v>
       </c>
       <c r="F4">
-        <v>201160.5025564647</v>
+        <v>201160.5025564648</v>
       </c>
       <c r="G4">
         <v>206748.866861733</v>
@@ -739,7 +739,7 @@
         <v>19160.30242512919</v>
       </c>
       <c r="H5">
-        <v>26165.95440800995</v>
+        <v>26165.95440800994</v>
       </c>
       <c r="I5">
         <v>28752.27800424531</v>
@@ -824,7 +824,7 @@
         <v>17960.1781240045</v>
       </c>
       <c r="K7">
-        <v>17960.17812400449</v>
+        <v>17960.1781240045</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -1055,7 +1055,7 @@
         <v>0</v>
       </c>
       <c r="L13">
-        <v>9615.869225027169</v>
+        <v>9615.869225027167</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1078,10 +1078,10 @@
         <v>4769.284525849926</v>
       </c>
       <c r="G14">
-        <v>8428.673142576763</v>
+        <v>8428.673142576761</v>
       </c>
       <c r="H14">
-        <v>8625.014163091058</v>
+        <v>8625.014163091062</v>
       </c>
       <c r="I14">
         <v>8704.992482561125</v>
@@ -1090,7 +1090,7 @@
         <v>8430.976782247228</v>
       </c>
       <c r="K14">
-        <v>9125.711862047974</v>
+        <v>9125.711862047981</v>
       </c>
       <c r="L14">
         <v>506.0983802645876</v>
@@ -1125,7 +1125,7 @@
         <v>559.096692149867</v>
       </c>
       <c r="J15">
-        <v>1220.571203849674</v>
+        <v>1220.571203849673</v>
       </c>
       <c r="K15">
         <v>896.0952868267118</v>
@@ -1186,10 +1186,10 @@
         <v>78.29765381649612</v>
       </c>
       <c r="E17">
-        <v>96.69685293076805</v>
+        <v>96.69685293076806</v>
       </c>
       <c r="F17">
-        <v>158.5983795893451</v>
+        <v>158.598379589345</v>
       </c>
       <c r="G17">
         <v>106.0922944805327</v>
@@ -1198,10 +1198,10 @@
         <v>358.637905790592</v>
       </c>
       <c r="I17">
-        <v>591.2027189729818</v>
+        <v>591.2027189729815</v>
       </c>
       <c r="J17">
-        <v>1365.022408251164</v>
+        <v>1365.022408251165</v>
       </c>
       <c r="K17">
         <v>221.5567571181343</v>
@@ -1230,19 +1230,19 @@
         <v>0</v>
       </c>
       <c r="G18">
-        <v>53.04614724026638</v>
+        <v>53.04614724026636</v>
       </c>
       <c r="H18">
         <v>330.3243869123872</v>
       </c>
       <c r="I18">
-        <v>971.8400859829836</v>
+        <v>971.8400859829837</v>
       </c>
       <c r="J18">
         <v>1242.001733978597</v>
       </c>
       <c r="K18">
-        <v>2351.214565335303</v>
+        <v>2351.214565335304</v>
       </c>
       <c r="L18">
         <v>0</v>
@@ -1303,10 +1303,10 @@
         <v>0.08164598301763558</v>
       </c>
       <c r="F20">
+        <v>0.09732201175702154</v>
+      </c>
+      <c r="G20">
         <v>0.09732201175702156</v>
-      </c>
-      <c r="G20">
-        <v>0.09732201175702154</v>
       </c>
       <c r="H20">
         <v>0.605486610058785</v>
@@ -1508,10 +1508,10 @@
         <v>203.2274331820474</v>
       </c>
       <c r="K25">
-        <v>475.542107917297</v>
+        <v>475.5421079172971</v>
       </c>
       <c r="L25">
-        <v>746.3439233484618</v>
+        <v>746.3439233484619</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -1731,16 +1731,16 @@
         <v>8794.229787156315</v>
       </c>
       <c r="F3">
-        <v>9071.388231228389</v>
+        <v>9071.388231228388</v>
       </c>
       <c r="G3">
         <v>9627.87291842199</v>
       </c>
       <c r="H3">
-        <v>8686.894223305411</v>
+        <v>8686.894223305413</v>
       </c>
       <c r="I3">
-        <v>6275.088936836572</v>
+        <v>6275.088936836571</v>
       </c>
       <c r="J3">
         <v>4291.369658321681</v>
@@ -1778,13 +1778,13 @@
         <v>704.8464421353992</v>
       </c>
       <c r="I4">
-        <v>1310.698275604317</v>
+        <v>1310.698275604318</v>
       </c>
       <c r="J4">
         <v>1857.637384770093</v>
       </c>
       <c r="K4">
-        <v>2439.558564642701</v>
+        <v>2439.5585646427</v>
       </c>
       <c r="L4">
         <v>2883.555982152331</v>
@@ -1807,7 +1807,7 @@
         <v>3259.605335069284</v>
       </c>
       <c r="F5">
-        <v>2276.544131015129</v>
+        <v>2276.54413101513</v>
       </c>
       <c r="G5">
         <v>2367.835042203508</v>
@@ -1825,7 +1825,7 @@
         <v>12.75969221759952</v>
       </c>
       <c r="L5">
-        <v>3.180724233320471</v>
+        <v>3.18072423332047</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1889,19 +1889,19 @@
         <v>362.4329451308008</v>
       </c>
       <c r="H7">
-        <v>381.8449619024159</v>
+        <v>381.8449619024158</v>
       </c>
       <c r="I7">
         <v>398.9149312047225</v>
       </c>
       <c r="J7">
-        <v>416.2371346060165</v>
+        <v>416.2371346060166</v>
       </c>
       <c r="K7">
-        <v>431.8338026884384</v>
+        <v>431.8338026884385</v>
       </c>
       <c r="L7">
-        <v>444.8604762525726</v>
+        <v>444.8604762525727</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1965,16 +1965,16 @@
         <v>157.9836779882429</v>
       </c>
       <c r="H9">
-        <v>703.4715557703609</v>
+        <v>703.4715557703605</v>
       </c>
       <c r="I9">
-        <v>1610.417360662471</v>
+        <v>1610.41736066247</v>
       </c>
       <c r="J9">
-        <v>2710.269957595709</v>
+        <v>2710.26995759571</v>
       </c>
       <c r="K9">
-        <v>2698.173429859351</v>
+        <v>2698.17342985935</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -1997,10 +1997,10 @@
         <v>0.08164598301763558</v>
       </c>
       <c r="F10">
+        <v>0.09732201175702154</v>
+      </c>
+      <c r="G10">
         <v>0.09732201175702156</v>
-      </c>
-      <c r="G10">
-        <v>0.09732201175702154</v>
       </c>
       <c r="H10">
         <v>0.605486610058785</v>
@@ -2050,7 +2050,7 @@
         <v>0.3036104049143241</v>
       </c>
       <c r="K11">
-        <v>16.89497844925109</v>
+        <v>16.89497844925108</v>
       </c>
       <c r="L11">
         <v>1.203604884863263</v>
@@ -2079,19 +2079,19 @@
         <v>0</v>
       </c>
       <c r="H12">
-        <v>0.007838014369693008</v>
+        <v>0.00783801436969301</v>
       </c>
       <c r="I12">
-        <v>1.634823134130165</v>
+        <v>1.634823134130164</v>
       </c>
       <c r="J12">
         <v>11.13647832356899</v>
       </c>
       <c r="K12">
-        <v>11.1286403091993</v>
+        <v>11.12864030919929</v>
       </c>
       <c r="L12">
-        <v>11.1286403091993</v>
+        <v>11.12864030919929</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -2117,10 +2117,10 @@
         <v>0</v>
       </c>
       <c r="H13">
-        <v>0.008705114254624596</v>
+        <v>0.008705114254624594</v>
       </c>
       <c r="I13">
-        <v>0.05404425099746102</v>
+        <v>0.05404425099746103</v>
       </c>
       <c r="J13">
         <v>0.3502764422252889</v>
@@ -2155,19 +2155,19 @@
         <v>0.2195780176643772</v>
       </c>
       <c r="H14">
-        <v>2.296365711102829</v>
+        <v>2.29636571110283</v>
       </c>
       <c r="I14">
-        <v>11.73004611093005</v>
+        <v>11.73004611093006</v>
       </c>
       <c r="J14">
-        <v>80.54890712129571</v>
+        <v>80.54890712129573</v>
       </c>
       <c r="K14">
-        <v>453.1249431839199</v>
+        <v>453.1249431839201</v>
       </c>
       <c r="L14">
-        <v>446.331315290568</v>
+        <v>446.3313152905681</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -2205,7 +2205,7 @@
         <v>0</v>
       </c>
       <c r="L15">
-        <v>415.5613815748115</v>
+        <v>415.5613815748114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>